<commit_message>
Updated to limit the number of cases to 100 to match the free tier
</commit_message>
<xml_diff>
--- a/Producer-Consumer_Cases.xlsx
+++ b/Producer-Consumer_Cases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tim/Documents/Webinars/June Webinar - Work Data Management/Work Data Management Bot/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tim/Documents/Webinars/June Webinar - Work Data Management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849A27F1-920D-9447-97BB-7D2CA6D8485F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E5852B-D215-A146-83FF-FB7287F9BC40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20180" xr2:uid="{88315F8B-3553-3948-BE34-B7233A7EDF9C}"/>
   </bookViews>
@@ -400,7 +400,7 @@
   <dimension ref="A1:J504"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1710,9 +1710,7 @@
       <c r="J101" s="2"/>
     </row>
     <row r="102" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A102" s="2">
-        <v>2124</v>
-      </c>
+      <c r="A102" s="2"/>
       <c r="B102" s="1"/>
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
@@ -1723,9 +1721,7 @@
       <c r="J102" s="2"/>
     </row>
     <row r="103" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A103" s="2">
-        <v>2125</v>
-      </c>
+      <c r="A103" s="2"/>
       <c r="B103" s="1"/>
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
@@ -1736,9 +1732,7 @@
       <c r="J103" s="2"/>
     </row>
     <row r="104" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A104" s="2">
-        <v>2126</v>
-      </c>
+      <c r="A104" s="2"/>
       <c r="B104" s="1"/>
       <c r="D104" s="2"/>
       <c r="E104" s="2"/>
@@ -1749,9 +1743,7 @@
       <c r="J104" s="2"/>
     </row>
     <row r="105" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A105" s="2">
-        <v>2127</v>
-      </c>
+      <c r="A105" s="2"/>
       <c r="B105" s="1"/>
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
@@ -1762,9 +1754,7 @@
       <c r="J105" s="2"/>
     </row>
     <row r="106" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A106" s="2">
-        <v>2128</v>
-      </c>
+      <c r="A106" s="2"/>
       <c r="B106" s="1"/>
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
@@ -1775,9 +1765,7 @@
       <c r="J106" s="2"/>
     </row>
     <row r="107" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A107" s="2">
-        <v>2129</v>
-      </c>
+      <c r="A107" s="2"/>
       <c r="B107" s="1"/>
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
@@ -1788,9 +1776,7 @@
       <c r="J107" s="2"/>
     </row>
     <row r="108" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A108" s="2">
-        <v>2130</v>
-      </c>
+      <c r="A108" s="2"/>
       <c r="B108" s="1"/>
       <c r="D108" s="2"/>
       <c r="E108" s="2"/>
@@ -1801,9 +1787,7 @@
       <c r="J108" s="2"/>
     </row>
     <row r="109" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A109" s="2">
-        <v>2131</v>
-      </c>
+      <c r="A109" s="2"/>
       <c r="B109" s="1"/>
       <c r="D109" s="2"/>
       <c r="E109" s="2"/>
@@ -1814,9 +1798,7 @@
       <c r="J109" s="2"/>
     </row>
     <row r="110" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A110" s="2">
-        <v>2132</v>
-      </c>
+      <c r="A110" s="2"/>
       <c r="B110" s="1"/>
       <c r="D110" s="2"/>
       <c r="E110" s="2"/>
@@ -1827,9 +1809,7 @@
       <c r="J110" s="2"/>
     </row>
     <row r="111" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A111" s="2">
-        <v>2133</v>
-      </c>
+      <c r="A111" s="2"/>
       <c r="B111" s="1"/>
       <c r="D111" s="2"/>
       <c r="E111" s="2"/>
@@ -1840,9 +1820,7 @@
       <c r="J111" s="2"/>
     </row>
     <row r="112" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A112" s="2">
-        <v>2134</v>
-      </c>
+      <c r="A112" s="2"/>
       <c r="B112" s="1"/>
       <c r="D112" s="2"/>
       <c r="E112" s="2"/>
@@ -1853,9 +1831,7 @@
       <c r="J112" s="2"/>
     </row>
     <row r="113" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A113" s="2">
-        <v>2135</v>
-      </c>
+      <c r="A113" s="2"/>
       <c r="B113" s="1"/>
       <c r="D113" s="2"/>
       <c r="E113" s="2"/>
@@ -1866,9 +1842,7 @@
       <c r="J113" s="2"/>
     </row>
     <row r="114" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A114" s="2">
-        <v>2136</v>
-      </c>
+      <c r="A114" s="2"/>
       <c r="B114" s="1"/>
       <c r="D114" s="2"/>
       <c r="E114" s="2"/>
@@ -1879,9 +1853,7 @@
       <c r="J114" s="2"/>
     </row>
     <row r="115" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A115" s="2">
-        <v>2137</v>
-      </c>
+      <c r="A115" s="2"/>
       <c r="B115" s="1"/>
       <c r="D115" s="2"/>
       <c r="E115" s="2"/>
@@ -1892,9 +1864,7 @@
       <c r="J115" s="2"/>
     </row>
     <row r="116" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A116" s="2">
-        <v>2138</v>
-      </c>
+      <c r="A116" s="2"/>
       <c r="B116" s="1"/>
       <c r="D116" s="2"/>
       <c r="E116" s="2"/>
@@ -1905,9 +1875,7 @@
       <c r="J116" s="2"/>
     </row>
     <row r="117" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A117" s="2">
-        <v>2139</v>
-      </c>
+      <c r="A117" s="2"/>
       <c r="B117" s="1"/>
       <c r="D117" s="2"/>
       <c r="E117" s="2"/>
@@ -1918,9 +1886,7 @@
       <c r="J117" s="2"/>
     </row>
     <row r="118" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A118" s="2">
-        <v>2140</v>
-      </c>
+      <c r="A118" s="2"/>
       <c r="B118" s="1"/>
       <c r="D118" s="2"/>
       <c r="E118" s="2"/>
@@ -1931,9 +1897,7 @@
       <c r="J118" s="2"/>
     </row>
     <row r="119" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A119" s="2">
-        <v>2141</v>
-      </c>
+      <c r="A119" s="2"/>
       <c r="B119" s="1"/>
       <c r="D119" s="2"/>
       <c r="E119" s="2"/>
@@ -1944,9 +1908,7 @@
       <c r="J119" s="2"/>
     </row>
     <row r="120" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A120" s="2">
-        <v>2142</v>
-      </c>
+      <c r="A120" s="2"/>
       <c r="B120" s="1"/>
       <c r="D120" s="2"/>
       <c r="E120" s="2"/>
@@ -1957,9 +1919,7 @@
       <c r="J120" s="2"/>
     </row>
     <row r="121" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A121" s="2">
-        <v>2143</v>
-      </c>
+      <c r="A121" s="2"/>
       <c r="B121" s="1"/>
       <c r="D121" s="2"/>
       <c r="E121" s="2"/>
@@ -1970,9 +1930,7 @@
       <c r="J121" s="2"/>
     </row>
     <row r="122" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A122" s="2">
-        <v>2144</v>
-      </c>
+      <c r="A122" s="2"/>
       <c r="B122" s="1"/>
       <c r="D122" s="2"/>
       <c r="E122" s="2"/>
@@ -1983,9 +1941,7 @@
       <c r="J122" s="2"/>
     </row>
     <row r="123" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A123" s="2">
-        <v>2145</v>
-      </c>
+      <c r="A123" s="2"/>
       <c r="B123" s="1"/>
       <c r="D123" s="2"/>
       <c r="E123" s="2"/>
@@ -1996,9 +1952,7 @@
       <c r="J123" s="2"/>
     </row>
     <row r="124" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A124" s="2">
-        <v>2146</v>
-      </c>
+      <c r="A124" s="2"/>
       <c r="B124" s="1"/>
       <c r="D124" s="2"/>
       <c r="E124" s="2"/>
@@ -2009,9 +1963,7 @@
       <c r="J124" s="2"/>
     </row>
     <row r="125" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A125" s="2">
-        <v>2147</v>
-      </c>
+      <c r="A125" s="2"/>
       <c r="B125" s="1"/>
       <c r="D125" s="2"/>
       <c r="E125" s="2"/>
@@ -2022,9 +1974,7 @@
       <c r="J125" s="2"/>
     </row>
     <row r="126" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A126" s="2">
-        <v>2148</v>
-      </c>
+      <c r="A126" s="2"/>
       <c r="B126" s="1"/>
       <c r="D126" s="2"/>
       <c r="E126" s="2"/>
@@ -2035,9 +1985,7 @@
       <c r="J126" s="2"/>
     </row>
     <row r="127" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A127" s="2">
-        <v>2149</v>
-      </c>
+      <c r="A127" s="2"/>
       <c r="B127" s="1"/>
       <c r="D127" s="2"/>
       <c r="E127" s="2"/>
@@ -2048,9 +1996,7 @@
       <c r="J127" s="2"/>
     </row>
     <row r="128" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A128" s="2">
-        <v>2150</v>
-      </c>
+      <c r="A128" s="2"/>
       <c r="B128" s="1"/>
       <c r="D128" s="2"/>
       <c r="E128" s="2"/>
@@ -2061,9 +2007,7 @@
       <c r="J128" s="2"/>
     </row>
     <row r="129" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A129" s="2">
-        <v>2151</v>
-      </c>
+      <c r="A129" s="2"/>
       <c r="B129" s="1"/>
       <c r="D129" s="2"/>
       <c r="E129" s="2"/>
@@ -2074,9 +2018,7 @@
       <c r="J129" s="2"/>
     </row>
     <row r="130" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A130" s="2">
-        <v>2152</v>
-      </c>
+      <c r="A130" s="2"/>
       <c r="B130" s="1"/>
       <c r="D130" s="2"/>
       <c r="E130" s="2"/>
@@ -2087,9 +2029,7 @@
       <c r="J130" s="2"/>
     </row>
     <row r="131" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A131" s="2">
-        <v>2153</v>
-      </c>
+      <c r="A131" s="2"/>
       <c r="B131" s="1"/>
       <c r="D131" s="2"/>
       <c r="E131" s="2"/>
@@ -2100,9 +2040,7 @@
       <c r="J131" s="2"/>
     </row>
     <row r="132" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A132" s="2">
-        <v>2154</v>
-      </c>
+      <c r="A132" s="2"/>
       <c r="B132" s="1"/>
       <c r="D132" s="2"/>
       <c r="E132" s="2"/>
@@ -2113,9 +2051,7 @@
       <c r="J132" s="2"/>
     </row>
     <row r="133" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A133" s="2">
-        <v>2155</v>
-      </c>
+      <c r="A133" s="2"/>
       <c r="B133" s="1"/>
       <c r="D133" s="2"/>
       <c r="E133" s="2"/>
@@ -2126,9 +2062,7 @@
       <c r="J133" s="2"/>
     </row>
     <row r="134" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A134" s="2">
-        <v>2156</v>
-      </c>
+      <c r="A134" s="2"/>
       <c r="B134" s="1"/>
       <c r="D134" s="2"/>
       <c r="E134" s="2"/>
@@ -2139,9 +2073,7 @@
       <c r="J134" s="2"/>
     </row>
     <row r="135" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A135" s="2">
-        <v>2157</v>
-      </c>
+      <c r="A135" s="2"/>
       <c r="B135" s="1"/>
       <c r="D135" s="2"/>
       <c r="E135" s="2"/>
@@ -2152,9 +2084,7 @@
       <c r="J135" s="2"/>
     </row>
     <row r="136" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A136" s="2">
-        <v>2158</v>
-      </c>
+      <c r="A136" s="2"/>
       <c r="B136" s="1"/>
       <c r="D136" s="2"/>
       <c r="E136" s="2"/>
@@ -2165,9 +2095,7 @@
       <c r="J136" s="2"/>
     </row>
     <row r="137" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A137" s="2">
-        <v>2159</v>
-      </c>
+      <c r="A137" s="2"/>
       <c r="B137" s="1"/>
       <c r="D137" s="2"/>
       <c r="E137" s="2"/>
@@ -2178,9 +2106,7 @@
       <c r="J137" s="2"/>
     </row>
     <row r="138" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A138" s="2">
-        <v>2160</v>
-      </c>
+      <c r="A138" s="2"/>
       <c r="B138" s="1"/>
       <c r="D138" s="2"/>
       <c r="E138" s="2"/>
@@ -2191,9 +2117,7 @@
       <c r="J138" s="2"/>
     </row>
     <row r="139" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A139" s="2">
-        <v>2161</v>
-      </c>
+      <c r="A139" s="2"/>
       <c r="B139" s="1"/>
       <c r="D139" s="2"/>
       <c r="E139" s="2"/>
@@ -2204,9 +2128,7 @@
       <c r="J139" s="2"/>
     </row>
     <row r="140" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A140" s="2">
-        <v>2162</v>
-      </c>
+      <c r="A140" s="2"/>
       <c r="B140" s="1"/>
       <c r="D140" s="2"/>
       <c r="E140" s="2"/>
@@ -2217,9 +2139,7 @@
       <c r="J140" s="2"/>
     </row>
     <row r="141" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A141" s="2">
-        <v>2163</v>
-      </c>
+      <c r="A141" s="2"/>
       <c r="B141" s="1"/>
       <c r="D141" s="2"/>
       <c r="E141" s="2"/>
@@ -2230,9 +2150,7 @@
       <c r="J141" s="2"/>
     </row>
     <row r="142" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A142" s="2">
-        <v>2164</v>
-      </c>
+      <c r="A142" s="2"/>
       <c r="B142" s="1"/>
       <c r="D142" s="2"/>
       <c r="E142" s="2"/>
@@ -2243,9 +2161,7 @@
       <c r="J142" s="2"/>
     </row>
     <row r="143" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A143" s="2">
-        <v>2165</v>
-      </c>
+      <c r="A143" s="2"/>
       <c r="B143" s="1"/>
       <c r="D143" s="2"/>
       <c r="E143" s="2"/>
@@ -2256,9 +2172,7 @@
       <c r="J143" s="2"/>
     </row>
     <row r="144" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A144" s="2">
-        <v>2166</v>
-      </c>
+      <c r="A144" s="2"/>
       <c r="B144" s="1"/>
       <c r="D144" s="2"/>
       <c r="E144" s="2"/>
@@ -2269,9 +2183,7 @@
       <c r="J144" s="2"/>
     </row>
     <row r="145" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A145" s="2">
-        <v>2167</v>
-      </c>
+      <c r="A145" s="2"/>
       <c r="B145" s="1"/>
       <c r="D145" s="2"/>
       <c r="E145" s="2"/>
@@ -2282,9 +2194,7 @@
       <c r="J145" s="2"/>
     </row>
     <row r="146" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A146" s="2">
-        <v>2168</v>
-      </c>
+      <c r="A146" s="2"/>
       <c r="B146" s="1"/>
       <c r="D146" s="2"/>
       <c r="E146" s="2"/>
@@ -2295,9 +2205,7 @@
       <c r="J146" s="2"/>
     </row>
     <row r="147" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A147" s="2">
-        <v>2169</v>
-      </c>
+      <c r="A147" s="2"/>
       <c r="B147" s="1"/>
       <c r="D147" s="2"/>
       <c r="E147" s="2"/>
@@ -2308,9 +2216,7 @@
       <c r="J147" s="2"/>
     </row>
     <row r="148" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A148" s="2">
-        <v>2170</v>
-      </c>
+      <c r="A148" s="2"/>
       <c r="B148" s="1"/>
       <c r="D148" s="2"/>
       <c r="E148" s="2"/>
@@ -2321,9 +2227,7 @@
       <c r="J148" s="2"/>
     </row>
     <row r="149" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A149" s="2">
-        <v>2171</v>
-      </c>
+      <c r="A149" s="2"/>
       <c r="B149" s="1"/>
       <c r="D149" s="2"/>
       <c r="E149" s="2"/>
@@ -2334,9 +2238,7 @@
       <c r="J149" s="2"/>
     </row>
     <row r="150" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A150" s="2">
-        <v>2172</v>
-      </c>
+      <c r="A150" s="2"/>
       <c r="B150" s="1"/>
       <c r="D150" s="2"/>
       <c r="E150" s="2"/>
@@ -2347,9 +2249,7 @@
       <c r="J150" s="2"/>
     </row>
     <row r="151" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A151" s="2">
-        <v>2173</v>
-      </c>
+      <c r="A151" s="2"/>
       <c r="B151" s="1"/>
       <c r="D151" s="2"/>
       <c r="E151" s="2"/>
@@ -2360,9 +2260,7 @@
       <c r="J151" s="2"/>
     </row>
     <row r="152" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A152" s="2">
-        <v>2174</v>
-      </c>
+      <c r="A152" s="2"/>
       <c r="B152" s="1"/>
       <c r="D152" s="2"/>
       <c r="E152" s="2"/>
@@ -2373,9 +2271,7 @@
       <c r="J152" s="2"/>
     </row>
     <row r="153" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A153" s="2">
-        <v>2175</v>
-      </c>
+      <c r="A153" s="2"/>
       <c r="B153" s="1"/>
       <c r="D153" s="2"/>
       <c r="E153" s="2"/>
@@ -2386,9 +2282,7 @@
       <c r="J153" s="2"/>
     </row>
     <row r="154" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A154" s="2">
-        <v>2176</v>
-      </c>
+      <c r="A154" s="2"/>
       <c r="B154" s="1"/>
       <c r="D154" s="2"/>
       <c r="E154" s="2"/>
@@ -2399,9 +2293,7 @@
       <c r="J154" s="2"/>
     </row>
     <row r="155" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A155" s="2">
-        <v>2177</v>
-      </c>
+      <c r="A155" s="2"/>
       <c r="B155" s="1"/>
       <c r="D155" s="2"/>
       <c r="E155" s="2"/>
@@ -2412,9 +2304,7 @@
       <c r="J155" s="2"/>
     </row>
     <row r="156" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A156" s="2">
-        <v>2178</v>
-      </c>
+      <c r="A156" s="2"/>
       <c r="B156" s="1"/>
       <c r="D156" s="2"/>
       <c r="E156" s="2"/>
@@ -2425,9 +2315,7 @@
       <c r="J156" s="2"/>
     </row>
     <row r="157" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A157" s="2">
-        <v>2179</v>
-      </c>
+      <c r="A157" s="2"/>
       <c r="B157" s="1"/>
       <c r="D157" s="2"/>
       <c r="E157" s="2"/>
@@ -2438,9 +2326,7 @@
       <c r="J157" s="2"/>
     </row>
     <row r="158" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A158" s="2">
-        <v>2180</v>
-      </c>
+      <c r="A158" s="2"/>
       <c r="B158" s="1"/>
       <c r="D158" s="2"/>
       <c r="E158" s="2"/>
@@ -2451,9 +2337,7 @@
       <c r="J158" s="2"/>
     </row>
     <row r="159" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A159" s="2">
-        <v>2181</v>
-      </c>
+      <c r="A159" s="2"/>
       <c r="B159" s="1"/>
       <c r="D159" s="2"/>
       <c r="E159" s="2"/>
@@ -2464,9 +2348,7 @@
       <c r="J159" s="2"/>
     </row>
     <row r="160" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A160" s="2">
-        <v>2182</v>
-      </c>
+      <c r="A160" s="2"/>
       <c r="B160" s="1"/>
       <c r="D160" s="2"/>
       <c r="E160" s="2"/>
@@ -2477,9 +2359,7 @@
       <c r="J160" s="2"/>
     </row>
     <row r="161" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A161" s="2">
-        <v>2183</v>
-      </c>
+      <c r="A161" s="2"/>
       <c r="B161" s="1"/>
       <c r="D161" s="2"/>
       <c r="E161" s="2"/>
@@ -2490,9 +2370,7 @@
       <c r="J161" s="2"/>
     </row>
     <row r="162" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A162" s="2">
-        <v>2184</v>
-      </c>
+      <c r="A162" s="2"/>
       <c r="B162" s="1"/>
       <c r="D162" s="2"/>
       <c r="E162" s="2"/>
@@ -2503,9 +2381,7 @@
       <c r="J162" s="2"/>
     </row>
     <row r="163" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A163" s="2">
-        <v>2185</v>
-      </c>
+      <c r="A163" s="2"/>
       <c r="B163" s="1"/>
       <c r="D163" s="2"/>
       <c r="E163" s="2"/>
@@ -2516,9 +2392,7 @@
       <c r="J163" s="2"/>
     </row>
     <row r="164" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A164" s="2">
-        <v>2186</v>
-      </c>
+      <c r="A164" s="2"/>
       <c r="B164" s="1"/>
       <c r="D164" s="2"/>
       <c r="E164" s="2"/>
@@ -2529,9 +2403,7 @@
       <c r="J164" s="2"/>
     </row>
     <row r="165" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A165" s="2">
-        <v>2187</v>
-      </c>
+      <c r="A165" s="2"/>
       <c r="B165" s="1"/>
       <c r="D165" s="2"/>
       <c r="E165" s="2"/>
@@ -2542,9 +2414,7 @@
       <c r="J165" s="2"/>
     </row>
     <row r="166" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A166" s="2">
-        <v>2188</v>
-      </c>
+      <c r="A166" s="2"/>
       <c r="B166" s="1"/>
       <c r="D166" s="2"/>
       <c r="E166" s="2"/>
@@ -2555,9 +2425,7 @@
       <c r="J166" s="2"/>
     </row>
     <row r="167" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A167" s="2">
-        <v>2189</v>
-      </c>
+      <c r="A167" s="2"/>
       <c r="B167" s="1"/>
       <c r="D167" s="2"/>
       <c r="E167" s="2"/>
@@ -2568,9 +2436,7 @@
       <c r="J167" s="2"/>
     </row>
     <row r="168" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A168" s="2">
-        <v>2190</v>
-      </c>
+      <c r="A168" s="2"/>
       <c r="B168" s="1"/>
       <c r="D168" s="2"/>
       <c r="E168" s="2"/>
@@ -2581,9 +2447,7 @@
       <c r="J168" s="2"/>
     </row>
     <row r="169" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A169" s="2">
-        <v>2191</v>
-      </c>
+      <c r="A169" s="2"/>
       <c r="B169" s="1"/>
       <c r="D169" s="2"/>
       <c r="E169" s="2"/>
@@ -2594,9 +2458,7 @@
       <c r="J169" s="2"/>
     </row>
     <row r="170" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A170" s="2">
-        <v>2192</v>
-      </c>
+      <c r="A170" s="2"/>
       <c r="B170" s="1"/>
       <c r="D170" s="2"/>
       <c r="E170" s="2"/>
@@ -2607,9 +2469,7 @@
       <c r="J170" s="2"/>
     </row>
     <row r="171" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A171" s="2">
-        <v>2193</v>
-      </c>
+      <c r="A171" s="2"/>
       <c r="B171" s="1"/>
       <c r="D171" s="2"/>
       <c r="E171" s="2"/>
@@ -2620,9 +2480,7 @@
       <c r="J171" s="2"/>
     </row>
     <row r="172" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A172" s="2">
-        <v>2194</v>
-      </c>
+      <c r="A172" s="2"/>
       <c r="B172" s="1"/>
       <c r="D172" s="2"/>
       <c r="E172" s="2"/>
@@ -2633,9 +2491,7 @@
       <c r="J172" s="2"/>
     </row>
     <row r="173" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A173" s="2">
-        <v>2195</v>
-      </c>
+      <c r="A173" s="2"/>
       <c r="B173" s="1"/>
       <c r="D173" s="2"/>
       <c r="E173" s="2"/>
@@ -2646,9 +2502,7 @@
       <c r="J173" s="2"/>
     </row>
     <row r="174" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A174" s="2">
-        <v>2196</v>
-      </c>
+      <c r="A174" s="2"/>
       <c r="B174" s="1"/>
       <c r="D174" s="2"/>
       <c r="E174" s="2"/>
@@ -2659,9 +2513,7 @@
       <c r="J174" s="2"/>
     </row>
     <row r="175" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A175" s="2">
-        <v>2197</v>
-      </c>
+      <c r="A175" s="2"/>
       <c r="B175" s="1"/>
       <c r="D175" s="2"/>
       <c r="E175" s="2"/>
@@ -2672,9 +2524,7 @@
       <c r="J175" s="2"/>
     </row>
     <row r="176" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A176" s="2">
-        <v>2198</v>
-      </c>
+      <c r="A176" s="2"/>
       <c r="B176" s="1"/>
       <c r="D176" s="2"/>
       <c r="E176" s="2"/>
@@ -2685,9 +2535,7 @@
       <c r="J176" s="2"/>
     </row>
     <row r="177" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A177" s="2">
-        <v>2199</v>
-      </c>
+      <c r="A177" s="2"/>
       <c r="B177" s="1"/>
       <c r="D177" s="2"/>
       <c r="E177" s="2"/>
@@ -2698,9 +2546,7 @@
       <c r="J177" s="2"/>
     </row>
     <row r="178" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A178" s="2">
-        <v>2200</v>
-      </c>
+      <c r="A178" s="2"/>
       <c r="B178" s="1"/>
       <c r="D178" s="2"/>
       <c r="E178" s="2"/>
@@ -2711,9 +2557,7 @@
       <c r="J178" s="2"/>
     </row>
     <row r="179" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A179" s="2">
-        <v>2201</v>
-      </c>
+      <c r="A179" s="2"/>
       <c r="B179" s="1"/>
       <c r="D179" s="2"/>
       <c r="E179" s="2"/>
@@ -2724,9 +2568,7 @@
       <c r="J179" s="2"/>
     </row>
     <row r="180" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A180" s="2">
-        <v>2202</v>
-      </c>
+      <c r="A180" s="2"/>
       <c r="B180" s="1"/>
       <c r="D180" s="2"/>
       <c r="E180" s="2"/>
@@ -2737,9 +2579,7 @@
       <c r="J180" s="2"/>
     </row>
     <row r="181" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A181" s="2">
-        <v>2203</v>
-      </c>
+      <c r="A181" s="2"/>
       <c r="B181" s="1"/>
       <c r="D181" s="2"/>
       <c r="E181" s="2"/>
@@ -2750,9 +2590,7 @@
       <c r="J181" s="2"/>
     </row>
     <row r="182" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A182" s="2">
-        <v>2204</v>
-      </c>
+      <c r="A182" s="2"/>
       <c r="B182" s="1"/>
       <c r="D182" s="2"/>
       <c r="E182" s="2"/>
@@ -2763,9 +2601,7 @@
       <c r="J182" s="2"/>
     </row>
     <row r="183" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A183" s="2">
-        <v>2205</v>
-      </c>
+      <c r="A183" s="2"/>
       <c r="B183" s="1"/>
       <c r="D183" s="2"/>
       <c r="E183" s="2"/>
@@ -2776,9 +2612,7 @@
       <c r="J183" s="2"/>
     </row>
     <row r="184" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A184" s="2">
-        <v>2206</v>
-      </c>
+      <c r="A184" s="2"/>
       <c r="B184" s="1"/>
       <c r="D184" s="2"/>
       <c r="E184" s="2"/>
@@ -2789,9 +2623,7 @@
       <c r="J184" s="2"/>
     </row>
     <row r="185" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A185" s="2">
-        <v>2207</v>
-      </c>
+      <c r="A185" s="2"/>
       <c r="B185" s="1"/>
       <c r="D185" s="2"/>
       <c r="E185" s="2"/>
@@ -2802,9 +2634,7 @@
       <c r="J185" s="2"/>
     </row>
     <row r="186" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A186" s="2">
-        <v>2208</v>
-      </c>
+      <c r="A186" s="2"/>
       <c r="B186" s="1"/>
       <c r="D186" s="2"/>
       <c r="E186" s="2"/>
@@ -2815,9 +2645,7 @@
       <c r="J186" s="2"/>
     </row>
     <row r="187" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A187" s="2">
-        <v>2209</v>
-      </c>
+      <c r="A187" s="2"/>
       <c r="B187" s="1"/>
       <c r="D187" s="2"/>
       <c r="E187" s="2"/>
@@ -2828,9 +2656,7 @@
       <c r="J187" s="2"/>
     </row>
     <row r="188" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A188" s="2">
-        <v>2210</v>
-      </c>
+      <c r="A188" s="2"/>
       <c r="B188" s="1"/>
       <c r="D188" s="2"/>
       <c r="E188" s="2"/>
@@ -2841,9 +2667,7 @@
       <c r="J188" s="2"/>
     </row>
     <row r="189" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A189" s="2">
-        <v>2211</v>
-      </c>
+      <c r="A189" s="2"/>
       <c r="B189" s="1"/>
       <c r="D189" s="2"/>
       <c r="E189" s="2"/>
@@ -2854,9 +2678,7 @@
       <c r="J189" s="2"/>
     </row>
     <row r="190" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A190" s="2">
-        <v>2212</v>
-      </c>
+      <c r="A190" s="2"/>
       <c r="B190" s="1"/>
       <c r="D190" s="2"/>
       <c r="E190" s="2"/>
@@ -2867,9 +2689,7 @@
       <c r="J190" s="2"/>
     </row>
     <row r="191" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A191" s="2">
-        <v>2213</v>
-      </c>
+      <c r="A191" s="2"/>
       <c r="B191" s="1"/>
       <c r="D191" s="2"/>
       <c r="E191" s="2"/>
@@ -2880,9 +2700,7 @@
       <c r="J191" s="2"/>
     </row>
     <row r="192" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A192" s="2">
-        <v>2214</v>
-      </c>
+      <c r="A192" s="2"/>
       <c r="B192" s="1"/>
       <c r="D192" s="2"/>
       <c r="E192" s="2"/>
@@ -2893,9 +2711,7 @@
       <c r="J192" s="2"/>
     </row>
     <row r="193" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A193" s="2">
-        <v>2215</v>
-      </c>
+      <c r="A193" s="2"/>
       <c r="B193" s="1"/>
       <c r="D193" s="2"/>
       <c r="E193" s="2"/>
@@ -2906,9 +2722,7 @@
       <c r="J193" s="2"/>
     </row>
     <row r="194" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A194" s="2">
-        <v>2216</v>
-      </c>
+      <c r="A194" s="2"/>
       <c r="B194" s="1"/>
       <c r="D194" s="2"/>
       <c r="E194" s="2"/>
@@ -2919,9 +2733,7 @@
       <c r="J194" s="2"/>
     </row>
     <row r="195" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A195" s="2">
-        <v>2217</v>
-      </c>
+      <c r="A195" s="2"/>
       <c r="B195" s="1"/>
       <c r="D195" s="2"/>
       <c r="E195" s="2"/>
@@ -2932,9 +2744,7 @@
       <c r="J195" s="2"/>
     </row>
     <row r="196" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A196" s="2">
-        <v>2218</v>
-      </c>
+      <c r="A196" s="2"/>
       <c r="B196" s="1"/>
       <c r="D196" s="2"/>
       <c r="E196" s="2"/>
@@ -2945,9 +2755,7 @@
       <c r="J196" s="2"/>
     </row>
     <row r="197" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A197" s="2">
-        <v>2219</v>
-      </c>
+      <c r="A197" s="2"/>
       <c r="B197" s="1"/>
       <c r="D197" s="2"/>
       <c r="E197" s="2"/>
@@ -2958,9 +2766,7 @@
       <c r="J197" s="2"/>
     </row>
     <row r="198" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A198" s="2">
-        <v>2220</v>
-      </c>
+      <c r="A198" s="2"/>
       <c r="B198" s="1"/>
       <c r="D198" s="2"/>
       <c r="E198" s="2"/>
@@ -2971,9 +2777,7 @@
       <c r="J198" s="2"/>
     </row>
     <row r="199" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A199" s="2">
-        <v>2221</v>
-      </c>
+      <c r="A199" s="2"/>
       <c r="B199" s="1"/>
       <c r="D199" s="2"/>
       <c r="E199" s="2"/>
@@ -2984,9 +2788,7 @@
       <c r="J199" s="2"/>
     </row>
     <row r="200" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A200" s="2">
-        <v>2222</v>
-      </c>
+      <c r="A200" s="2"/>
       <c r="B200" s="1"/>
       <c r="D200" s="2"/>
       <c r="E200" s="2"/>
@@ -2997,9 +2799,7 @@
       <c r="J200" s="2"/>
     </row>
     <row r="201" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A201" s="2">
-        <v>2223</v>
-      </c>
+      <c r="A201" s="2"/>
       <c r="B201" s="1"/>
       <c r="D201" s="2"/>
       <c r="E201" s="2"/>
@@ -3010,9 +2810,7 @@
       <c r="J201" s="2"/>
     </row>
     <row r="202" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A202" s="2">
-        <v>2224</v>
-      </c>
+      <c r="A202" s="2"/>
       <c r="B202" s="1"/>
       <c r="D202" s="2"/>
       <c r="E202" s="2"/>
@@ -3023,9 +2821,7 @@
       <c r="J202" s="2"/>
     </row>
     <row r="203" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A203" s="2">
-        <v>2225</v>
-      </c>
+      <c r="A203" s="2"/>
       <c r="B203" s="1"/>
       <c r="D203" s="2"/>
       <c r="E203" s="2"/>
@@ -3036,9 +2832,7 @@
       <c r="J203" s="2"/>
     </row>
     <row r="204" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A204" s="2">
-        <v>2226</v>
-      </c>
+      <c r="A204" s="2"/>
       <c r="B204" s="1"/>
       <c r="D204" s="2"/>
       <c r="E204" s="2"/>
@@ -3049,9 +2843,7 @@
       <c r="J204" s="2"/>
     </row>
     <row r="205" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A205" s="2">
-        <v>2227</v>
-      </c>
+      <c r="A205" s="2"/>
       <c r="B205" s="1"/>
       <c r="D205" s="2"/>
       <c r="E205" s="2"/>
@@ -3062,9 +2854,7 @@
       <c r="J205" s="2"/>
     </row>
     <row r="206" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A206" s="2">
-        <v>2228</v>
-      </c>
+      <c r="A206" s="2"/>
       <c r="B206" s="1"/>
       <c r="D206" s="2"/>
       <c r="E206" s="2"/>
@@ -3075,9 +2865,7 @@
       <c r="J206" s="2"/>
     </row>
     <row r="207" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A207" s="2">
-        <v>2229</v>
-      </c>
+      <c r="A207" s="2"/>
       <c r="B207" s="1"/>
       <c r="D207" s="2"/>
       <c r="E207" s="2"/>
@@ -3088,9 +2876,7 @@
       <c r="J207" s="2"/>
     </row>
     <row r="208" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A208" s="2">
-        <v>2230</v>
-      </c>
+      <c r="A208" s="2"/>
       <c r="B208" s="1"/>
       <c r="D208" s="2"/>
       <c r="E208" s="2"/>
@@ -3101,9 +2887,7 @@
       <c r="J208" s="2"/>
     </row>
     <row r="209" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A209" s="2">
-        <v>2231</v>
-      </c>
+      <c r="A209" s="2"/>
       <c r="B209" s="1"/>
       <c r="D209" s="2"/>
       <c r="E209" s="2"/>
@@ -3114,9 +2898,7 @@
       <c r="J209" s="2"/>
     </row>
     <row r="210" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A210" s="2">
-        <v>2232</v>
-      </c>
+      <c r="A210" s="2"/>
       <c r="B210" s="1"/>
       <c r="D210" s="2"/>
       <c r="E210" s="2"/>
@@ -3127,9 +2909,7 @@
       <c r="J210" s="2"/>
     </row>
     <row r="211" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A211" s="2">
-        <v>2233</v>
-      </c>
+      <c r="A211" s="2"/>
       <c r="B211" s="1"/>
       <c r="D211" s="2"/>
       <c r="E211" s="2"/>
@@ -3140,9 +2920,7 @@
       <c r="J211" s="2"/>
     </row>
     <row r="212" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A212" s="2">
-        <v>2234</v>
-      </c>
+      <c r="A212" s="2"/>
       <c r="B212" s="1"/>
       <c r="D212" s="2"/>
       <c r="E212" s="2"/>
@@ -3153,9 +2931,7 @@
       <c r="J212" s="2"/>
     </row>
     <row r="213" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A213" s="2">
-        <v>2235</v>
-      </c>
+      <c r="A213" s="2"/>
       <c r="B213" s="1"/>
       <c r="D213" s="2"/>
       <c r="E213" s="2"/>
@@ -3166,9 +2942,7 @@
       <c r="J213" s="2"/>
     </row>
     <row r="214" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A214" s="2">
-        <v>2236</v>
-      </c>
+      <c r="A214" s="2"/>
       <c r="B214" s="1"/>
       <c r="D214" s="2"/>
       <c r="E214" s="2"/>
@@ -3179,9 +2953,7 @@
       <c r="J214" s="2"/>
     </row>
     <row r="215" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A215" s="2">
-        <v>2237</v>
-      </c>
+      <c r="A215" s="2"/>
       <c r="B215" s="1"/>
       <c r="D215" s="2"/>
       <c r="E215" s="2"/>
@@ -3192,9 +2964,7 @@
       <c r="J215" s="2"/>
     </row>
     <row r="216" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A216" s="2">
-        <v>2238</v>
-      </c>
+      <c r="A216" s="2"/>
       <c r="B216" s="1"/>
       <c r="D216" s="2"/>
       <c r="E216" s="2"/>
@@ -3205,9 +2975,7 @@
       <c r="J216" s="2"/>
     </row>
     <row r="217" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A217" s="2">
-        <v>2239</v>
-      </c>
+      <c r="A217" s="2"/>
       <c r="B217" s="1"/>
       <c r="D217" s="2"/>
       <c r="E217" s="2"/>
@@ -3218,9 +2986,7 @@
       <c r="J217" s="2"/>
     </row>
     <row r="218" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A218" s="2">
-        <v>2240</v>
-      </c>
+      <c r="A218" s="2"/>
       <c r="B218" s="1"/>
       <c r="D218" s="2"/>
       <c r="E218" s="2"/>
@@ -3231,9 +2997,7 @@
       <c r="J218" s="2"/>
     </row>
     <row r="219" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A219" s="2">
-        <v>2241</v>
-      </c>
+      <c r="A219" s="2"/>
       <c r="B219" s="1"/>
       <c r="D219" s="2"/>
       <c r="E219" s="2"/>
@@ -3244,9 +3008,7 @@
       <c r="J219" s="2"/>
     </row>
     <row r="220" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A220" s="2">
-        <v>2242</v>
-      </c>
+      <c r="A220" s="2"/>
       <c r="B220" s="1"/>
       <c r="D220" s="2"/>
       <c r="E220" s="2"/>
@@ -3257,9 +3019,7 @@
       <c r="J220" s="2"/>
     </row>
     <row r="221" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A221" s="2">
-        <v>2243</v>
-      </c>
+      <c r="A221" s="2"/>
       <c r="B221" s="1"/>
       <c r="D221" s="2"/>
       <c r="E221" s="2"/>
@@ -3270,9 +3030,7 @@
       <c r="J221" s="2"/>
     </row>
     <row r="222" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A222" s="2">
-        <v>2244</v>
-      </c>
+      <c r="A222" s="2"/>
       <c r="B222" s="1"/>
       <c r="D222" s="2"/>
       <c r="E222" s="2"/>
@@ -3283,9 +3041,7 @@
       <c r="J222" s="2"/>
     </row>
     <row r="223" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A223" s="2">
-        <v>2245</v>
-      </c>
+      <c r="A223" s="2"/>
       <c r="B223" s="1"/>
       <c r="D223" s="2"/>
       <c r="E223" s="2"/>
@@ -3296,9 +3052,7 @@
       <c r="J223" s="2"/>
     </row>
     <row r="224" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A224" s="2">
-        <v>2246</v>
-      </c>
+      <c r="A224" s="2"/>
       <c r="B224" s="1"/>
       <c r="D224" s="2"/>
       <c r="E224" s="2"/>
@@ -3309,9 +3063,7 @@
       <c r="J224" s="2"/>
     </row>
     <row r="225" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A225" s="2">
-        <v>2247</v>
-      </c>
+      <c r="A225" s="2"/>
       <c r="B225" s="1"/>
       <c r="D225" s="2"/>
       <c r="E225" s="2"/>
@@ -3322,9 +3074,7 @@
       <c r="J225" s="2"/>
     </row>
     <row r="226" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A226" s="2">
-        <v>2248</v>
-      </c>
+      <c r="A226" s="2"/>
       <c r="B226" s="1"/>
       <c r="D226" s="2"/>
       <c r="E226" s="2"/>
@@ -3335,9 +3085,7 @@
       <c r="J226" s="2"/>
     </row>
     <row r="227" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A227" s="2">
-        <v>2249</v>
-      </c>
+      <c r="A227" s="2"/>
       <c r="B227" s="1"/>
       <c r="D227" s="2"/>
       <c r="E227" s="2"/>
@@ -3348,9 +3096,7 @@
       <c r="J227" s="2"/>
     </row>
     <row r="228" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A228" s="2">
-        <v>2250</v>
-      </c>
+      <c r="A228" s="2"/>
       <c r="B228" s="1"/>
       <c r="D228" s="2"/>
       <c r="E228" s="2"/>
@@ -3361,9 +3107,7 @@
       <c r="J228" s="2"/>
     </row>
     <row r="229" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A229" s="2">
-        <v>2251</v>
-      </c>
+      <c r="A229" s="2"/>
       <c r="B229" s="1"/>
       <c r="D229" s="2"/>
       <c r="E229" s="2"/>
@@ -3374,9 +3118,7 @@
       <c r="J229" s="2"/>
     </row>
     <row r="230" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A230" s="2">
-        <v>2252</v>
-      </c>
+      <c r="A230" s="2"/>
       <c r="B230" s="1"/>
       <c r="D230" s="2"/>
       <c r="E230" s="2"/>
@@ -3387,9 +3129,7 @@
       <c r="J230" s="2"/>
     </row>
     <row r="231" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A231" s="2">
-        <v>2253</v>
-      </c>
+      <c r="A231" s="2"/>
       <c r="B231" s="1"/>
       <c r="D231" s="2"/>
       <c r="E231" s="2"/>
@@ -3400,9 +3140,7 @@
       <c r="J231" s="2"/>
     </row>
     <row r="232" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A232" s="2">
-        <v>2254</v>
-      </c>
+      <c r="A232" s="2"/>
       <c r="B232" s="1"/>
       <c r="D232" s="2"/>
       <c r="E232" s="2"/>
@@ -3413,9 +3151,7 @@
       <c r="J232" s="2"/>
     </row>
     <row r="233" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A233" s="2">
-        <v>2255</v>
-      </c>
+      <c r="A233" s="2"/>
       <c r="B233" s="1"/>
       <c r="D233" s="2"/>
       <c r="E233" s="2"/>
@@ -3426,9 +3162,7 @@
       <c r="J233" s="2"/>
     </row>
     <row r="234" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A234" s="2">
-        <v>2256</v>
-      </c>
+      <c r="A234" s="2"/>
       <c r="B234" s="1"/>
       <c r="D234" s="2"/>
       <c r="E234" s="2"/>
@@ -3439,9 +3173,7 @@
       <c r="J234" s="2"/>
     </row>
     <row r="235" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A235" s="2">
-        <v>2257</v>
-      </c>
+      <c r="A235" s="2"/>
       <c r="B235" s="1"/>
       <c r="D235" s="2"/>
       <c r="E235" s="2"/>
@@ -3452,9 +3184,7 @@
       <c r="J235" s="2"/>
     </row>
     <row r="236" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A236" s="2">
-        <v>2258</v>
-      </c>
+      <c r="A236" s="2"/>
       <c r="B236" s="1"/>
       <c r="D236" s="2"/>
       <c r="E236" s="2"/>
@@ -3465,9 +3195,7 @@
       <c r="J236" s="2"/>
     </row>
     <row r="237" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A237" s="2">
-        <v>2259</v>
-      </c>
+      <c r="A237" s="2"/>
       <c r="B237" s="1"/>
       <c r="D237" s="2"/>
       <c r="E237" s="2"/>
@@ -3478,9 +3206,7 @@
       <c r="J237" s="2"/>
     </row>
     <row r="238" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A238" s="2">
-        <v>2260</v>
-      </c>
+      <c r="A238" s="2"/>
       <c r="B238" s="1"/>
       <c r="D238" s="2"/>
       <c r="E238" s="2"/>
@@ -3491,9 +3217,7 @@
       <c r="J238" s="2"/>
     </row>
     <row r="239" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A239" s="2">
-        <v>2261</v>
-      </c>
+      <c r="A239" s="2"/>
       <c r="B239" s="1"/>
       <c r="D239" s="2"/>
       <c r="E239" s="2"/>
@@ -3504,9 +3228,7 @@
       <c r="J239" s="2"/>
     </row>
     <row r="240" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A240" s="2">
-        <v>2262</v>
-      </c>
+      <c r="A240" s="2"/>
       <c r="B240" s="1"/>
       <c r="D240" s="2"/>
       <c r="E240" s="2"/>
@@ -3517,9 +3239,7 @@
       <c r="J240" s="2"/>
     </row>
     <row r="241" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A241" s="2">
-        <v>2263</v>
-      </c>
+      <c r="A241" s="2"/>
       <c r="B241" s="1"/>
       <c r="D241" s="2"/>
       <c r="E241" s="2"/>
@@ -3530,9 +3250,7 @@
       <c r="J241" s="2"/>
     </row>
     <row r="242" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A242" s="2">
-        <v>2264</v>
-      </c>
+      <c r="A242" s="2"/>
       <c r="B242" s="1"/>
       <c r="D242" s="2"/>
       <c r="E242" s="2"/>
@@ -3543,9 +3261,7 @@
       <c r="J242" s="2"/>
     </row>
     <row r="243" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A243" s="2">
-        <v>2265</v>
-      </c>
+      <c r="A243" s="2"/>
       <c r="B243" s="1"/>
       <c r="D243" s="2"/>
       <c r="E243" s="2"/>
@@ -3556,9 +3272,7 @@
       <c r="J243" s="2"/>
     </row>
     <row r="244" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A244" s="2">
-        <v>2266</v>
-      </c>
+      <c r="A244" s="2"/>
       <c r="B244" s="1"/>
       <c r="D244" s="2"/>
       <c r="E244" s="2"/>
@@ -3569,9 +3283,7 @@
       <c r="J244" s="2"/>
     </row>
     <row r="245" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A245" s="2">
-        <v>2267</v>
-      </c>
+      <c r="A245" s="2"/>
       <c r="B245" s="1"/>
       <c r="D245" s="2"/>
       <c r="E245" s="2"/>
@@ -3582,9 +3294,7 @@
       <c r="J245" s="2"/>
     </row>
     <row r="246" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A246" s="2">
-        <v>2268</v>
-      </c>
+      <c r="A246" s="2"/>
       <c r="B246" s="1"/>
       <c r="D246" s="2"/>
       <c r="E246" s="2"/>
@@ -3595,9 +3305,7 @@
       <c r="J246" s="2"/>
     </row>
     <row r="247" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A247" s="2">
-        <v>2269</v>
-      </c>
+      <c r="A247" s="2"/>
       <c r="B247" s="1"/>
       <c r="D247" s="2"/>
       <c r="E247" s="2"/>
@@ -3608,9 +3316,7 @@
       <c r="J247" s="2"/>
     </row>
     <row r="248" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A248" s="2">
-        <v>2270</v>
-      </c>
+      <c r="A248" s="2"/>
       <c r="B248" s="1"/>
       <c r="D248" s="2"/>
       <c r="E248" s="2"/>
@@ -3621,9 +3327,7 @@
       <c r="J248" s="2"/>
     </row>
     <row r="249" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A249" s="2">
-        <v>2271</v>
-      </c>
+      <c r="A249" s="2"/>
       <c r="B249" s="1"/>
       <c r="D249" s="2"/>
       <c r="E249" s="2"/>
@@ -3634,9 +3338,7 @@
       <c r="J249" s="2"/>
     </row>
     <row r="250" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A250" s="2">
-        <v>2272</v>
-      </c>
+      <c r="A250" s="2"/>
       <c r="B250" s="1"/>
       <c r="D250" s="2"/>
       <c r="E250" s="2"/>
@@ -3647,9 +3349,7 @@
       <c r="J250" s="2"/>
     </row>
     <row r="251" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A251" s="2">
-        <v>2273</v>
-      </c>
+      <c r="A251" s="2"/>
       <c r="B251" s="1"/>
       <c r="D251" s="2"/>
       <c r="E251" s="2"/>
@@ -3660,9 +3360,7 @@
       <c r="J251" s="2"/>
     </row>
     <row r="252" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A252" s="2">
-        <v>2274</v>
-      </c>
+      <c r="A252" s="2"/>
       <c r="B252" s="1"/>
       <c r="D252" s="2"/>
       <c r="E252" s="2"/>
@@ -3673,9 +3371,7 @@
       <c r="J252" s="2"/>
     </row>
     <row r="253" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A253" s="2">
-        <v>2275</v>
-      </c>
+      <c r="A253" s="2"/>
       <c r="B253" s="1"/>
       <c r="D253" s="2"/>
       <c r="E253" s="2"/>
@@ -3686,9 +3382,7 @@
       <c r="J253" s="2"/>
     </row>
     <row r="254" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A254" s="2">
-        <v>2276</v>
-      </c>
+      <c r="A254" s="2"/>
       <c r="B254" s="1"/>
       <c r="D254" s="2"/>
       <c r="E254" s="2"/>
@@ -3699,9 +3393,7 @@
       <c r="J254" s="2"/>
     </row>
     <row r="255" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A255" s="2">
-        <v>2277</v>
-      </c>
+      <c r="A255" s="2"/>
       <c r="B255" s="1"/>
       <c r="D255" s="2"/>
       <c r="E255" s="2"/>
@@ -3712,9 +3404,7 @@
       <c r="J255" s="2"/>
     </row>
     <row r="256" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A256" s="2">
-        <v>2278</v>
-      </c>
+      <c r="A256" s="2"/>
       <c r="B256" s="1"/>
       <c r="D256" s="2"/>
       <c r="E256" s="2"/>
@@ -3725,9 +3415,7 @@
       <c r="J256" s="2"/>
     </row>
     <row r="257" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A257" s="2">
-        <v>2279</v>
-      </c>
+      <c r="A257" s="2"/>
       <c r="B257" s="1"/>
       <c r="D257" s="2"/>
       <c r="E257" s="2"/>
@@ -3738,9 +3426,7 @@
       <c r="J257" s="2"/>
     </row>
     <row r="258" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A258" s="2">
-        <v>2280</v>
-      </c>
+      <c r="A258" s="2"/>
       <c r="B258" s="1"/>
       <c r="D258" s="2"/>
       <c r="E258" s="2"/>
@@ -3751,9 +3437,7 @@
       <c r="J258" s="2"/>
     </row>
     <row r="259" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A259" s="2">
-        <v>2281</v>
-      </c>
+      <c r="A259" s="2"/>
       <c r="B259" s="1"/>
       <c r="D259" s="2"/>
       <c r="E259" s="2"/>
@@ -3764,9 +3448,7 @@
       <c r="J259" s="2"/>
     </row>
     <row r="260" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A260" s="2">
-        <v>2282</v>
-      </c>
+      <c r="A260" s="2"/>
       <c r="B260" s="1"/>
       <c r="D260" s="2"/>
       <c r="E260" s="2"/>
@@ -3777,9 +3459,7 @@
       <c r="J260" s="2"/>
     </row>
     <row r="261" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A261" s="2">
-        <v>2283</v>
-      </c>
+      <c r="A261" s="2"/>
       <c r="B261" s="1"/>
       <c r="D261" s="2"/>
       <c r="E261" s="2"/>
@@ -3790,9 +3470,7 @@
       <c r="J261" s="2"/>
     </row>
     <row r="262" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A262" s="2">
-        <v>2284</v>
-      </c>
+      <c r="A262" s="2"/>
       <c r="B262" s="1"/>
       <c r="D262" s="2"/>
       <c r="E262" s="2"/>
@@ -3803,9 +3481,7 @@
       <c r="J262" s="2"/>
     </row>
     <row r="263" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A263" s="2">
-        <v>2285</v>
-      </c>
+      <c r="A263" s="2"/>
       <c r="B263" s="1"/>
       <c r="D263" s="2"/>
       <c r="E263" s="2"/>
@@ -3816,9 +3492,7 @@
       <c r="J263" s="2"/>
     </row>
     <row r="264" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A264" s="2">
-        <v>2286</v>
-      </c>
+      <c r="A264" s="2"/>
       <c r="B264" s="1"/>
       <c r="D264" s="2"/>
       <c r="E264" s="2"/>
@@ -3829,9 +3503,7 @@
       <c r="J264" s="2"/>
     </row>
     <row r="265" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A265" s="2">
-        <v>2287</v>
-      </c>
+      <c r="A265" s="2"/>
       <c r="B265" s="1"/>
       <c r="D265" s="2"/>
       <c r="E265" s="2"/>
@@ -3842,9 +3514,7 @@
       <c r="J265" s="2"/>
     </row>
     <row r="266" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A266" s="2">
-        <v>2288</v>
-      </c>
+      <c r="A266" s="2"/>
       <c r="B266" s="1"/>
       <c r="D266" s="2"/>
       <c r="E266" s="2"/>
@@ -3855,9 +3525,7 @@
       <c r="J266" s="2"/>
     </row>
     <row r="267" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A267" s="2">
-        <v>2289</v>
-      </c>
+      <c r="A267" s="2"/>
       <c r="B267" s="1"/>
       <c r="D267" s="2"/>
       <c r="E267" s="2"/>
@@ -3868,9 +3536,7 @@
       <c r="J267" s="2"/>
     </row>
     <row r="268" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A268" s="2">
-        <v>2290</v>
-      </c>
+      <c r="A268" s="2"/>
       <c r="B268" s="1"/>
       <c r="D268" s="2"/>
       <c r="E268" s="2"/>
@@ -3881,9 +3547,7 @@
       <c r="J268" s="2"/>
     </row>
     <row r="269" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A269" s="2">
-        <v>2291</v>
-      </c>
+      <c r="A269" s="2"/>
       <c r="B269" s="1"/>
       <c r="D269" s="2"/>
       <c r="E269" s="2"/>
@@ -3894,9 +3558,7 @@
       <c r="J269" s="2"/>
     </row>
     <row r="270" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A270" s="2">
-        <v>2292</v>
-      </c>
+      <c r="A270" s="2"/>
       <c r="B270" s="1"/>
       <c r="D270" s="2"/>
       <c r="E270" s="2"/>
@@ -3907,9 +3569,7 @@
       <c r="J270" s="2"/>
     </row>
     <row r="271" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A271" s="2">
-        <v>2293</v>
-      </c>
+      <c r="A271" s="2"/>
       <c r="B271" s="1"/>
       <c r="D271" s="2"/>
       <c r="E271" s="2"/>
@@ -3920,9 +3580,7 @@
       <c r="J271" s="2"/>
     </row>
     <row r="272" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A272" s="2">
-        <v>2294</v>
-      </c>
+      <c r="A272" s="2"/>
       <c r="B272" s="1"/>
       <c r="D272" s="2"/>
       <c r="E272" s="2"/>
@@ -3933,9 +3591,7 @@
       <c r="J272" s="2"/>
     </row>
     <row r="273" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A273" s="2">
-        <v>2295</v>
-      </c>
+      <c r="A273" s="2"/>
       <c r="B273" s="1"/>
       <c r="D273" s="2"/>
       <c r="E273" s="2"/>
@@ -3946,9 +3602,7 @@
       <c r="J273" s="2"/>
     </row>
     <row r="274" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A274" s="2">
-        <v>2296</v>
-      </c>
+      <c r="A274" s="2"/>
       <c r="B274" s="1"/>
       <c r="D274" s="2"/>
       <c r="E274" s="2"/>
@@ -3959,9 +3613,7 @@
       <c r="J274" s="2"/>
     </row>
     <row r="275" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A275" s="2">
-        <v>2297</v>
-      </c>
+      <c r="A275" s="2"/>
       <c r="B275" s="1"/>
       <c r="D275" s="2"/>
       <c r="E275" s="2"/>
@@ -3972,9 +3624,7 @@
       <c r="J275" s="2"/>
     </row>
     <row r="276" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A276" s="2">
-        <v>2298</v>
-      </c>
+      <c r="A276" s="2"/>
       <c r="B276" s="1"/>
       <c r="D276" s="2"/>
       <c r="E276" s="2"/>
@@ -3985,9 +3635,7 @@
       <c r="J276" s="2"/>
     </row>
     <row r="277" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A277" s="2">
-        <v>2299</v>
-      </c>
+      <c r="A277" s="2"/>
       <c r="B277" s="1"/>
       <c r="D277" s="2"/>
       <c r="E277" s="2"/>
@@ -3998,9 +3646,7 @@
       <c r="J277" s="2"/>
     </row>
     <row r="278" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A278" s="2">
-        <v>2300</v>
-      </c>
+      <c r="A278" s="2"/>
       <c r="B278" s="1"/>
       <c r="D278" s="2"/>
       <c r="E278" s="2"/>
@@ -4011,9 +3657,7 @@
       <c r="J278" s="2"/>
     </row>
     <row r="279" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A279" s="2">
-        <v>2301</v>
-      </c>
+      <c r="A279" s="2"/>
       <c r="B279" s="1"/>
       <c r="D279" s="2"/>
       <c r="E279" s="2"/>
@@ -4024,9 +3668,7 @@
       <c r="J279" s="2"/>
     </row>
     <row r="280" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A280" s="2">
-        <v>2302</v>
-      </c>
+      <c r="A280" s="2"/>
       <c r="B280" s="1"/>
       <c r="D280" s="2"/>
       <c r="E280" s="2"/>
@@ -4037,9 +3679,7 @@
       <c r="J280" s="2"/>
     </row>
     <row r="281" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A281" s="2">
-        <v>2303</v>
-      </c>
+      <c r="A281" s="2"/>
       <c r="B281" s="1"/>
       <c r="D281" s="2"/>
       <c r="E281" s="2"/>
@@ -4050,9 +3690,7 @@
       <c r="J281" s="2"/>
     </row>
     <row r="282" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A282" s="2">
-        <v>2304</v>
-      </c>
+      <c r="A282" s="2"/>
       <c r="B282" s="1"/>
       <c r="D282" s="2"/>
       <c r="E282" s="2"/>
@@ -4063,9 +3701,7 @@
       <c r="J282" s="2"/>
     </row>
     <row r="283" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A283" s="2">
-        <v>2305</v>
-      </c>
+      <c r="A283" s="2"/>
       <c r="B283" s="1"/>
       <c r="D283" s="2"/>
       <c r="E283" s="2"/>
@@ -4076,9 +3712,7 @@
       <c r="J283" s="2"/>
     </row>
     <row r="284" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A284" s="2">
-        <v>2306</v>
-      </c>
+      <c r="A284" s="2"/>
       <c r="B284" s="1"/>
       <c r="D284" s="2"/>
       <c r="E284" s="2"/>
@@ -4089,9 +3723,7 @@
       <c r="J284" s="2"/>
     </row>
     <row r="285" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A285" s="2">
-        <v>2307</v>
-      </c>
+      <c r="A285" s="2"/>
       <c r="B285" s="1"/>
       <c r="D285" s="2"/>
       <c r="E285" s="2"/>
@@ -4102,9 +3734,7 @@
       <c r="J285" s="2"/>
     </row>
     <row r="286" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A286" s="2">
-        <v>2308</v>
-      </c>
+      <c r="A286" s="2"/>
       <c r="B286" s="1"/>
       <c r="D286" s="2"/>
       <c r="E286" s="2"/>
@@ -4115,9 +3745,7 @@
       <c r="J286" s="2"/>
     </row>
     <row r="287" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A287" s="2">
-        <v>2309</v>
-      </c>
+      <c r="A287" s="2"/>
       <c r="B287" s="1"/>
       <c r="D287" s="2"/>
       <c r="E287" s="2"/>
@@ -4128,9 +3756,7 @@
       <c r="J287" s="2"/>
     </row>
     <row r="288" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A288" s="2">
-        <v>2310</v>
-      </c>
+      <c r="A288" s="2"/>
       <c r="B288" s="1"/>
       <c r="D288" s="2"/>
       <c r="E288" s="2"/>
@@ -4141,9 +3767,7 @@
       <c r="J288" s="2"/>
     </row>
     <row r="289" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A289" s="2">
-        <v>2311</v>
-      </c>
+      <c r="A289" s="2"/>
       <c r="B289" s="1"/>
       <c r="D289" s="2"/>
       <c r="E289" s="2"/>
@@ -4154,9 +3778,7 @@
       <c r="J289" s="2"/>
     </row>
     <row r="290" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A290" s="2">
-        <v>2312</v>
-      </c>
+      <c r="A290" s="2"/>
       <c r="B290" s="1"/>
       <c r="D290" s="2"/>
       <c r="E290" s="2"/>
@@ -4167,9 +3789,7 @@
       <c r="J290" s="2"/>
     </row>
     <row r="291" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A291" s="2">
-        <v>2313</v>
-      </c>
+      <c r="A291" s="2"/>
       <c r="B291" s="1"/>
       <c r="D291" s="2"/>
       <c r="E291" s="2"/>
@@ -4180,9 +3800,7 @@
       <c r="J291" s="2"/>
     </row>
     <row r="292" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A292" s="2">
-        <v>2314</v>
-      </c>
+      <c r="A292" s="2"/>
       <c r="B292" s="1"/>
       <c r="D292" s="2"/>
       <c r="E292" s="2"/>
@@ -4193,9 +3811,7 @@
       <c r="J292" s="2"/>
     </row>
     <row r="293" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A293" s="2">
-        <v>2315</v>
-      </c>
+      <c r="A293" s="2"/>
       <c r="B293" s="1"/>
       <c r="D293" s="2"/>
       <c r="E293" s="2"/>
@@ -4206,9 +3822,7 @@
       <c r="J293" s="2"/>
     </row>
     <row r="294" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A294" s="2">
-        <v>2316</v>
-      </c>
+      <c r="A294" s="2"/>
       <c r="B294" s="1"/>
       <c r="D294" s="2"/>
       <c r="E294" s="2"/>
@@ -4219,9 +3833,7 @@
       <c r="J294" s="2"/>
     </row>
     <row r="295" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A295" s="2">
-        <v>2317</v>
-      </c>
+      <c r="A295" s="2"/>
       <c r="B295" s="1"/>
       <c r="D295" s="2"/>
       <c r="E295" s="2"/>
@@ -4232,9 +3844,7 @@
       <c r="J295" s="2"/>
     </row>
     <row r="296" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A296" s="2">
-        <v>2318</v>
-      </c>
+      <c r="A296" s="2"/>
       <c r="B296" s="1"/>
       <c r="D296" s="2"/>
       <c r="E296" s="2"/>
@@ -4245,9 +3855,7 @@
       <c r="J296" s="2"/>
     </row>
     <row r="297" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A297" s="2">
-        <v>2319</v>
-      </c>
+      <c r="A297" s="2"/>
       <c r="B297" s="1"/>
       <c r="D297" s="2"/>
       <c r="E297" s="2"/>
@@ -4258,9 +3866,7 @@
       <c r="J297" s="2"/>
     </row>
     <row r="298" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A298" s="2">
-        <v>2320</v>
-      </c>
+      <c r="A298" s="2"/>
       <c r="B298" s="1"/>
       <c r="D298" s="2"/>
       <c r="E298" s="2"/>
@@ -4271,9 +3877,7 @@
       <c r="J298" s="2"/>
     </row>
     <row r="299" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A299" s="2">
-        <v>2321</v>
-      </c>
+      <c r="A299" s="2"/>
       <c r="B299" s="1"/>
       <c r="D299" s="2"/>
       <c r="E299" s="2"/>
@@ -4284,9 +3888,7 @@
       <c r="J299" s="2"/>
     </row>
     <row r="300" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A300" s="2">
-        <v>2322</v>
-      </c>
+      <c r="A300" s="2"/>
       <c r="B300" s="1"/>
       <c r="D300" s="2"/>
       <c r="E300" s="2"/>
@@ -4297,9 +3899,7 @@
       <c r="J300" s="2"/>
     </row>
     <row r="301" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A301" s="2">
-        <v>2323</v>
-      </c>
+      <c r="A301" s="2"/>
       <c r="B301" s="1"/>
       <c r="D301" s="2"/>
       <c r="E301" s="2"/>
@@ -4310,9 +3910,7 @@
       <c r="J301" s="2"/>
     </row>
     <row r="302" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A302" s="2">
-        <v>2324</v>
-      </c>
+      <c r="A302" s="2"/>
       <c r="B302" s="1"/>
       <c r="D302" s="2"/>
       <c r="E302" s="2"/>
@@ -4323,9 +3921,7 @@
       <c r="J302" s="2"/>
     </row>
     <row r="303" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A303" s="2">
-        <v>2325</v>
-      </c>
+      <c r="A303" s="2"/>
       <c r="B303" s="1"/>
       <c r="D303" s="2"/>
       <c r="E303" s="2"/>
@@ -4336,9 +3932,7 @@
       <c r="J303" s="2"/>
     </row>
     <row r="304" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A304" s="2">
-        <v>2326</v>
-      </c>
+      <c r="A304" s="2"/>
       <c r="B304" s="1"/>
       <c r="D304" s="2"/>
       <c r="E304" s="2"/>
@@ -4349,9 +3943,7 @@
       <c r="J304" s="2"/>
     </row>
     <row r="305" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A305" s="2">
-        <v>2327</v>
-      </c>
+      <c r="A305" s="2"/>
       <c r="B305" s="1"/>
       <c r="D305" s="2"/>
       <c r="E305" s="2"/>
@@ -4362,9 +3954,7 @@
       <c r="J305" s="2"/>
     </row>
     <row r="306" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A306" s="2">
-        <v>2328</v>
-      </c>
+      <c r="A306" s="2"/>
       <c r="B306" s="1"/>
       <c r="D306" s="2"/>
       <c r="E306" s="2"/>
@@ -4375,9 +3965,7 @@
       <c r="J306" s="2"/>
     </row>
     <row r="307" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A307" s="2">
-        <v>2329</v>
-      </c>
+      <c r="A307" s="2"/>
       <c r="B307" s="1"/>
       <c r="D307" s="2"/>
       <c r="E307" s="2"/>
@@ -4388,9 +3976,7 @@
       <c r="J307" s="2"/>
     </row>
     <row r="308" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A308" s="2">
-        <v>2330</v>
-      </c>
+      <c r="A308" s="2"/>
       <c r="B308" s="1"/>
       <c r="D308" s="2"/>
       <c r="E308" s="2"/>
@@ -4401,9 +3987,7 @@
       <c r="J308" s="2"/>
     </row>
     <row r="309" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A309" s="2">
-        <v>2331</v>
-      </c>
+      <c r="A309" s="2"/>
       <c r="B309" s="1"/>
       <c r="D309" s="2"/>
       <c r="E309" s="2"/>
@@ -4414,9 +3998,7 @@
       <c r="J309" s="2"/>
     </row>
     <row r="310" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A310" s="2">
-        <v>2332</v>
-      </c>
+      <c r="A310" s="2"/>
       <c r="B310" s="1"/>
       <c r="D310" s="2"/>
       <c r="E310" s="2"/>
@@ -4427,9 +4009,7 @@
       <c r="J310" s="2"/>
     </row>
     <row r="311" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A311" s="2">
-        <v>2333</v>
-      </c>
+      <c r="A311" s="2"/>
       <c r="B311" s="1"/>
       <c r="D311" s="2"/>
       <c r="E311" s="2"/>
@@ -4440,9 +4020,7 @@
       <c r="J311" s="2"/>
     </row>
     <row r="312" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A312" s="2">
-        <v>2334</v>
-      </c>
+      <c r="A312" s="2"/>
       <c r="B312" s="1"/>
       <c r="D312" s="2"/>
       <c r="E312" s="2"/>
@@ -4453,9 +4031,7 @@
       <c r="J312" s="2"/>
     </row>
     <row r="313" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A313" s="2">
-        <v>2335</v>
-      </c>
+      <c r="A313" s="2"/>
       <c r="B313" s="1"/>
       <c r="D313" s="2"/>
       <c r="E313" s="2"/>
@@ -4466,9 +4042,7 @@
       <c r="J313" s="2"/>
     </row>
     <row r="314" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A314" s="2">
-        <v>2336</v>
-      </c>
+      <c r="A314" s="2"/>
       <c r="B314" s="1"/>
       <c r="D314" s="2"/>
       <c r="E314" s="2"/>
@@ -4479,9 +4053,7 @@
       <c r="J314" s="2"/>
     </row>
     <row r="315" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A315" s="2">
-        <v>2337</v>
-      </c>
+      <c r="A315" s="2"/>
       <c r="B315" s="1"/>
       <c r="D315" s="2"/>
       <c r="E315" s="2"/>
@@ -4492,9 +4064,7 @@
       <c r="J315" s="2"/>
     </row>
     <row r="316" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A316" s="2">
-        <v>2338</v>
-      </c>
+      <c r="A316" s="2"/>
       <c r="B316" s="1"/>
       <c r="D316" s="2"/>
       <c r="E316" s="2"/>
@@ -4505,9 +4075,7 @@
       <c r="J316" s="2"/>
     </row>
     <row r="317" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A317" s="2">
-        <v>2339</v>
-      </c>
+      <c r="A317" s="2"/>
       <c r="B317" s="1"/>
       <c r="D317" s="2"/>
       <c r="E317" s="2"/>
@@ -4518,9 +4086,7 @@
       <c r="J317" s="2"/>
     </row>
     <row r="318" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A318" s="2">
-        <v>2340</v>
-      </c>
+      <c r="A318" s="2"/>
       <c r="B318" s="1"/>
       <c r="D318" s="2"/>
       <c r="E318" s="2"/>
@@ -4531,9 +4097,7 @@
       <c r="J318" s="2"/>
     </row>
     <row r="319" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A319" s="2">
-        <v>2341</v>
-      </c>
+      <c r="A319" s="2"/>
       <c r="B319" s="1"/>
       <c r="D319" s="2"/>
       <c r="E319" s="2"/>
@@ -4544,9 +4108,7 @@
       <c r="J319" s="2"/>
     </row>
     <row r="320" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A320" s="2">
-        <v>2342</v>
-      </c>
+      <c r="A320" s="2"/>
       <c r="B320" s="1"/>
       <c r="D320" s="2"/>
       <c r="E320" s="2"/>
@@ -4557,9 +4119,7 @@
       <c r="J320" s="2"/>
     </row>
     <row r="321" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A321" s="2">
-        <v>2343</v>
-      </c>
+      <c r="A321" s="2"/>
       <c r="B321" s="1"/>
       <c r="D321" s="2"/>
       <c r="E321" s="2"/>
@@ -4570,9 +4130,7 @@
       <c r="J321" s="2"/>
     </row>
     <row r="322" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A322" s="2">
-        <v>2344</v>
-      </c>
+      <c r="A322" s="2"/>
       <c r="B322" s="1"/>
       <c r="D322" s="2"/>
       <c r="E322" s="2"/>
@@ -4583,9 +4141,7 @@
       <c r="J322" s="2"/>
     </row>
     <row r="323" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A323" s="2">
-        <v>2345</v>
-      </c>
+      <c r="A323" s="2"/>
       <c r="B323" s="1"/>
       <c r="D323" s="2"/>
       <c r="E323" s="2"/>
@@ -4596,9 +4152,7 @@
       <c r="J323" s="2"/>
     </row>
     <row r="324" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A324" s="2">
-        <v>2346</v>
-      </c>
+      <c r="A324" s="2"/>
       <c r="B324" s="1"/>
       <c r="D324" s="2"/>
       <c r="E324" s="2"/>
@@ -4609,9 +4163,7 @@
       <c r="J324" s="2"/>
     </row>
     <row r="325" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A325" s="2">
-        <v>2347</v>
-      </c>
+      <c r="A325" s="2"/>
       <c r="B325" s="1"/>
       <c r="D325" s="2"/>
       <c r="E325" s="2"/>
@@ -4622,9 +4174,7 @@
       <c r="J325" s="2"/>
     </row>
     <row r="326" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A326" s="2">
-        <v>2348</v>
-      </c>
+      <c r="A326" s="2"/>
       <c r="B326" s="1"/>
       <c r="D326" s="2"/>
       <c r="E326" s="2"/>
@@ -4635,9 +4185,7 @@
       <c r="J326" s="2"/>
     </row>
     <row r="327" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A327" s="2">
-        <v>2349</v>
-      </c>
+      <c r="A327" s="2"/>
       <c r="B327" s="1"/>
       <c r="D327" s="2"/>
       <c r="E327" s="2"/>
@@ -4648,9 +4196,7 @@
       <c r="J327" s="2"/>
     </row>
     <row r="328" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A328" s="2">
-        <v>2350</v>
-      </c>
+      <c r="A328" s="2"/>
       <c r="B328" s="1"/>
       <c r="D328" s="2"/>
       <c r="E328" s="2"/>
@@ -4661,9 +4207,7 @@
       <c r="J328" s="2"/>
     </row>
     <row r="329" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A329" s="2">
-        <v>2351</v>
-      </c>
+      <c r="A329" s="2"/>
       <c r="B329" s="1"/>
       <c r="D329" s="2"/>
       <c r="E329" s="2"/>
@@ -4674,9 +4218,7 @@
       <c r="J329" s="2"/>
     </row>
     <row r="330" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A330" s="2">
-        <v>2352</v>
-      </c>
+      <c r="A330" s="2"/>
       <c r="B330" s="1"/>
       <c r="D330" s="2"/>
       <c r="E330" s="2"/>
@@ -4687,9 +4229,7 @@
       <c r="J330" s="2"/>
     </row>
     <row r="331" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A331" s="2">
-        <v>2353</v>
-      </c>
+      <c r="A331" s="2"/>
       <c r="B331" s="1"/>
       <c r="D331" s="2"/>
       <c r="E331" s="2"/>
@@ -4700,9 +4240,7 @@
       <c r="J331" s="2"/>
     </row>
     <row r="332" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A332" s="2">
-        <v>2354</v>
-      </c>
+      <c r="A332" s="2"/>
       <c r="B332" s="1"/>
       <c r="D332" s="2"/>
       <c r="E332" s="2"/>
@@ -4713,9 +4251,7 @@
       <c r="J332" s="2"/>
     </row>
     <row r="333" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A333" s="2">
-        <v>2355</v>
-      </c>
+      <c r="A333" s="2"/>
       <c r="B333" s="1"/>
       <c r="D333" s="2"/>
       <c r="E333" s="2"/>
@@ -4726,9 +4262,7 @@
       <c r="J333" s="2"/>
     </row>
     <row r="334" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A334" s="2">
-        <v>2356</v>
-      </c>
+      <c r="A334" s="2"/>
       <c r="B334" s="1"/>
       <c r="D334" s="2"/>
       <c r="E334" s="2"/>
@@ -4739,9 +4273,7 @@
       <c r="J334" s="2"/>
     </row>
     <row r="335" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A335" s="2">
-        <v>2357</v>
-      </c>
+      <c r="A335" s="2"/>
       <c r="B335" s="1"/>
       <c r="D335" s="2"/>
       <c r="E335" s="2"/>
@@ -4752,9 +4284,7 @@
       <c r="J335" s="2"/>
     </row>
     <row r="336" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A336" s="2">
-        <v>2358</v>
-      </c>
+      <c r="A336" s="2"/>
       <c r="B336" s="1"/>
       <c r="D336" s="2"/>
       <c r="E336" s="2"/>
@@ -4765,9 +4295,7 @@
       <c r="J336" s="2"/>
     </row>
     <row r="337" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A337" s="2">
-        <v>2359</v>
-      </c>
+      <c r="A337" s="2"/>
       <c r="B337" s="1"/>
       <c r="D337" s="2"/>
       <c r="E337" s="2"/>
@@ -4778,9 +4306,7 @@
       <c r="J337" s="2"/>
     </row>
     <row r="338" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A338" s="2">
-        <v>2360</v>
-      </c>
+      <c r="A338" s="2"/>
       <c r="B338" s="1"/>
       <c r="D338" s="2"/>
       <c r="E338" s="2"/>
@@ -4791,9 +4317,7 @@
       <c r="J338" s="2"/>
     </row>
     <row r="339" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A339" s="2">
-        <v>2361</v>
-      </c>
+      <c r="A339" s="2"/>
       <c r="B339" s="1"/>
       <c r="D339" s="2"/>
       <c r="E339" s="2"/>
@@ -4804,9 +4328,7 @@
       <c r="J339" s="2"/>
     </row>
     <row r="340" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A340" s="2">
-        <v>2362</v>
-      </c>
+      <c r="A340" s="2"/>
       <c r="B340" s="1"/>
       <c r="D340" s="2"/>
       <c r="E340" s="2"/>
@@ -4817,9 +4339,7 @@
       <c r="J340" s="2"/>
     </row>
     <row r="341" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A341" s="2">
-        <v>2363</v>
-      </c>
+      <c r="A341" s="2"/>
       <c r="B341" s="1"/>
       <c r="D341" s="2"/>
       <c r="E341" s="2"/>
@@ -4830,9 +4350,7 @@
       <c r="J341" s="2"/>
     </row>
     <row r="342" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A342" s="2">
-        <v>2364</v>
-      </c>
+      <c r="A342" s="2"/>
       <c r="B342" s="1"/>
       <c r="D342" s="2"/>
       <c r="E342" s="2"/>
@@ -4843,9 +4361,7 @@
       <c r="J342" s="2"/>
     </row>
     <row r="343" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A343" s="2">
-        <v>2365</v>
-      </c>
+      <c r="A343" s="2"/>
       <c r="B343" s="1"/>
       <c r="D343" s="2"/>
       <c r="E343" s="2"/>
@@ -4856,9 +4372,7 @@
       <c r="J343" s="2"/>
     </row>
     <row r="344" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A344" s="2">
-        <v>2366</v>
-      </c>
+      <c r="A344" s="2"/>
       <c r="B344" s="1"/>
       <c r="D344" s="2"/>
       <c r="E344" s="2"/>
@@ -4869,9 +4383,7 @@
       <c r="J344" s="2"/>
     </row>
     <row r="345" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A345" s="2">
-        <v>2367</v>
-      </c>
+      <c r="A345" s="2"/>
       <c r="B345" s="1"/>
       <c r="D345" s="2"/>
       <c r="E345" s="2"/>
@@ -4882,9 +4394,7 @@
       <c r="J345" s="2"/>
     </row>
     <row r="346" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A346" s="2">
-        <v>2368</v>
-      </c>
+      <c r="A346" s="2"/>
       <c r="B346" s="1"/>
       <c r="D346" s="2"/>
       <c r="E346" s="2"/>
@@ -4895,9 +4405,7 @@
       <c r="J346" s="2"/>
     </row>
     <row r="347" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A347" s="2">
-        <v>2369</v>
-      </c>
+      <c r="A347" s="2"/>
       <c r="B347" s="1"/>
       <c r="D347" s="2"/>
       <c r="E347" s="2"/>
@@ -4908,9 +4416,7 @@
       <c r="J347" s="2"/>
     </row>
     <row r="348" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A348" s="2">
-        <v>2370</v>
-      </c>
+      <c r="A348" s="2"/>
       <c r="B348" s="1"/>
       <c r="D348" s="2"/>
       <c r="E348" s="2"/>
@@ -4921,9 +4427,7 @@
       <c r="J348" s="2"/>
     </row>
     <row r="349" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A349" s="2">
-        <v>2371</v>
-      </c>
+      <c r="A349" s="2"/>
       <c r="B349" s="1"/>
       <c r="D349" s="2"/>
       <c r="E349" s="2"/>
@@ -4934,9 +4438,7 @@
       <c r="J349" s="2"/>
     </row>
     <row r="350" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A350" s="2">
-        <v>2372</v>
-      </c>
+      <c r="A350" s="2"/>
       <c r="B350" s="1"/>
       <c r="D350" s="2"/>
       <c r="E350" s="2"/>
@@ -4947,9 +4449,7 @@
       <c r="J350" s="2"/>
     </row>
     <row r="351" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A351" s="2">
-        <v>2373</v>
-      </c>
+      <c r="A351" s="2"/>
       <c r="B351" s="1"/>
       <c r="D351" s="2"/>
       <c r="E351" s="2"/>
@@ -4960,9 +4460,7 @@
       <c r="J351" s="2"/>
     </row>
     <row r="352" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A352" s="2">
-        <v>2374</v>
-      </c>
+      <c r="A352" s="2"/>
       <c r="B352" s="1"/>
       <c r="D352" s="2"/>
       <c r="E352" s="2"/>
@@ -4973,9 +4471,7 @@
       <c r="J352" s="2"/>
     </row>
     <row r="353" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A353" s="2">
-        <v>2375</v>
-      </c>
+      <c r="A353" s="2"/>
       <c r="B353" s="1"/>
       <c r="D353" s="2"/>
       <c r="E353" s="2"/>
@@ -4986,9 +4482,7 @@
       <c r="J353" s="2"/>
     </row>
     <row r="354" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A354" s="2">
-        <v>2376</v>
-      </c>
+      <c r="A354" s="2"/>
       <c r="B354" s="1"/>
       <c r="D354" s="2"/>
       <c r="E354" s="2"/>
@@ -4999,9 +4493,7 @@
       <c r="J354" s="2"/>
     </row>
     <row r="355" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A355" s="2">
-        <v>2377</v>
-      </c>
+      <c r="A355" s="2"/>
       <c r="B355" s="1"/>
       <c r="D355" s="2"/>
       <c r="E355" s="2"/>
@@ -5012,9 +4504,7 @@
       <c r="J355" s="2"/>
     </row>
     <row r="356" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A356" s="2">
-        <v>2378</v>
-      </c>
+      <c r="A356" s="2"/>
       <c r="B356" s="1"/>
       <c r="D356" s="2"/>
       <c r="E356" s="2"/>
@@ -5025,9 +4515,7 @@
       <c r="J356" s="2"/>
     </row>
     <row r="357" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A357" s="2">
-        <v>2379</v>
-      </c>
+      <c r="A357" s="2"/>
       <c r="B357" s="1"/>
       <c r="D357" s="2"/>
       <c r="E357" s="2"/>
@@ -5038,9 +4526,7 @@
       <c r="J357" s="2"/>
     </row>
     <row r="358" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A358" s="2">
-        <v>2380</v>
-      </c>
+      <c r="A358" s="2"/>
       <c r="B358" s="1"/>
       <c r="D358" s="2"/>
       <c r="E358" s="2"/>
@@ -5051,9 +4537,7 @@
       <c r="J358" s="2"/>
     </row>
     <row r="359" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A359" s="2">
-        <v>2381</v>
-      </c>
+      <c r="A359" s="2"/>
       <c r="B359" s="1"/>
       <c r="D359" s="2"/>
       <c r="E359" s="2"/>
@@ -5064,9 +4548,7 @@
       <c r="J359" s="2"/>
     </row>
     <row r="360" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A360" s="2">
-        <v>2382</v>
-      </c>
+      <c r="A360" s="2"/>
       <c r="B360" s="1"/>
       <c r="D360" s="2"/>
       <c r="E360" s="2"/>
@@ -5077,9 +4559,7 @@
       <c r="J360" s="2"/>
     </row>
     <row r="361" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A361" s="2">
-        <v>2383</v>
-      </c>
+      <c r="A361" s="2"/>
       <c r="B361" s="1"/>
       <c r="D361" s="2"/>
       <c r="E361" s="2"/>
@@ -5090,9 +4570,7 @@
       <c r="J361" s="2"/>
     </row>
     <row r="362" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A362" s="2">
-        <v>2384</v>
-      </c>
+      <c r="A362" s="2"/>
       <c r="B362" s="1"/>
       <c r="D362" s="2"/>
       <c r="E362" s="2"/>
@@ -5103,9 +4581,7 @@
       <c r="J362" s="2"/>
     </row>
     <row r="363" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A363" s="2">
-        <v>2385</v>
-      </c>
+      <c r="A363" s="2"/>
       <c r="B363" s="1"/>
       <c r="D363" s="2"/>
       <c r="E363" s="2"/>
@@ -5116,9 +4592,7 @@
       <c r="J363" s="2"/>
     </row>
     <row r="364" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A364" s="2">
-        <v>2386</v>
-      </c>
+      <c r="A364" s="2"/>
       <c r="B364" s="1"/>
       <c r="D364" s="2"/>
       <c r="E364" s="2"/>
@@ -5129,9 +4603,7 @@
       <c r="J364" s="2"/>
     </row>
     <row r="365" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A365" s="2">
-        <v>2387</v>
-      </c>
+      <c r="A365" s="2"/>
       <c r="B365" s="1"/>
       <c r="D365" s="2"/>
       <c r="E365" s="2"/>
@@ -5142,9 +4614,7 @@
       <c r="J365" s="2"/>
     </row>
     <row r="366" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A366" s="2">
-        <v>2388</v>
-      </c>
+      <c r="A366" s="2"/>
       <c r="B366" s="1"/>
       <c r="D366" s="2"/>
       <c r="E366" s="2"/>
@@ -5155,9 +4625,7 @@
       <c r="J366" s="2"/>
     </row>
     <row r="367" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A367" s="2">
-        <v>2389</v>
-      </c>
+      <c r="A367" s="2"/>
       <c r="B367" s="1"/>
       <c r="D367" s="2"/>
       <c r="E367" s="2"/>
@@ -5168,9 +4636,7 @@
       <c r="J367" s="2"/>
     </row>
     <row r="368" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A368" s="2">
-        <v>2390</v>
-      </c>
+      <c r="A368" s="2"/>
       <c r="B368" s="1"/>
       <c r="D368" s="2"/>
       <c r="E368" s="2"/>
@@ -5181,9 +4647,7 @@
       <c r="J368" s="2"/>
     </row>
     <row r="369" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A369" s="2">
-        <v>2391</v>
-      </c>
+      <c r="A369" s="2"/>
       <c r="B369" s="1"/>
       <c r="D369" s="2"/>
       <c r="E369" s="2"/>
@@ -5194,9 +4658,7 @@
       <c r="J369" s="2"/>
     </row>
     <row r="370" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A370" s="2">
-        <v>2392</v>
-      </c>
+      <c r="A370" s="2"/>
       <c r="B370" s="1"/>
       <c r="D370" s="2"/>
       <c r="E370" s="2"/>
@@ -5207,9 +4669,7 @@
       <c r="J370" s="2"/>
     </row>
     <row r="371" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A371" s="2">
-        <v>2393</v>
-      </c>
+      <c r="A371" s="2"/>
       <c r="B371" s="1"/>
       <c r="D371" s="2"/>
       <c r="E371" s="2"/>
@@ -5220,9 +4680,7 @@
       <c r="J371" s="2"/>
     </row>
     <row r="372" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A372" s="2">
-        <v>2394</v>
-      </c>
+      <c r="A372" s="2"/>
       <c r="B372" s="1"/>
       <c r="D372" s="2"/>
       <c r="E372" s="2"/>
@@ -5233,9 +4691,7 @@
       <c r="J372" s="2"/>
     </row>
     <row r="373" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A373" s="2">
-        <v>2395</v>
-      </c>
+      <c r="A373" s="2"/>
       <c r="B373" s="1"/>
       <c r="D373" s="2"/>
       <c r="E373" s="2"/>
@@ -5246,9 +4702,7 @@
       <c r="J373" s="2"/>
     </row>
     <row r="374" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A374" s="2">
-        <v>2396</v>
-      </c>
+      <c r="A374" s="2"/>
       <c r="B374" s="1"/>
       <c r="D374" s="2"/>
       <c r="E374" s="2"/>
@@ -5259,9 +4713,7 @@
       <c r="J374" s="2"/>
     </row>
     <row r="375" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A375" s="2">
-        <v>2397</v>
-      </c>
+      <c r="A375" s="2"/>
       <c r="B375" s="1"/>
       <c r="D375" s="2"/>
       <c r="E375" s="2"/>
@@ -5272,9 +4724,7 @@
       <c r="J375" s="2"/>
     </row>
     <row r="376" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A376" s="2">
-        <v>2398</v>
-      </c>
+      <c r="A376" s="2"/>
       <c r="B376" s="1"/>
       <c r="D376" s="2"/>
       <c r="E376" s="2"/>
@@ -5285,9 +4735,7 @@
       <c r="J376" s="2"/>
     </row>
     <row r="377" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A377" s="2">
-        <v>2399</v>
-      </c>
+      <c r="A377" s="2"/>
       <c r="B377" s="1"/>
       <c r="D377" s="2"/>
       <c r="E377" s="2"/>
@@ -5298,9 +4746,7 @@
       <c r="J377" s="2"/>
     </row>
     <row r="378" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A378" s="2">
-        <v>2400</v>
-      </c>
+      <c r="A378" s="2"/>
       <c r="B378" s="1"/>
       <c r="D378" s="2"/>
       <c r="E378" s="2"/>
@@ -5311,9 +4757,7 @@
       <c r="J378" s="2"/>
     </row>
     <row r="379" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A379" s="2">
-        <v>2401</v>
-      </c>
+      <c r="A379" s="2"/>
       <c r="B379" s="1"/>
       <c r="D379" s="2"/>
       <c r="E379" s="2"/>
@@ -5324,9 +4768,7 @@
       <c r="J379" s="2"/>
     </row>
     <row r="380" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A380" s="2">
-        <v>2402</v>
-      </c>
+      <c r="A380" s="2"/>
       <c r="B380" s="1"/>
       <c r="D380" s="2"/>
       <c r="E380" s="2"/>
@@ -5337,9 +4779,7 @@
       <c r="J380" s="2"/>
     </row>
     <row r="381" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A381" s="2">
-        <v>2403</v>
-      </c>
+      <c r="A381" s="2"/>
       <c r="B381" s="1"/>
       <c r="D381" s="2"/>
       <c r="E381" s="2"/>
@@ -5350,9 +4790,7 @@
       <c r="J381" s="2"/>
     </row>
     <row r="382" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A382" s="2">
-        <v>2404</v>
-      </c>
+      <c r="A382" s="2"/>
       <c r="B382" s="1"/>
       <c r="D382" s="2"/>
       <c r="E382" s="2"/>
@@ -5363,9 +4801,7 @@
       <c r="J382" s="2"/>
     </row>
     <row r="383" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A383" s="2">
-        <v>2405</v>
-      </c>
+      <c r="A383" s="2"/>
       <c r="B383" s="1"/>
       <c r="D383" s="2"/>
       <c r="E383" s="2"/>
@@ -5376,9 +4812,7 @@
       <c r="J383" s="2"/>
     </row>
     <row r="384" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A384" s="2">
-        <v>2406</v>
-      </c>
+      <c r="A384" s="2"/>
       <c r="B384" s="1"/>
       <c r="D384" s="2"/>
       <c r="E384" s="2"/>
@@ -5389,9 +4823,7 @@
       <c r="J384" s="2"/>
     </row>
     <row r="385" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A385" s="2">
-        <v>2407</v>
-      </c>
+      <c r="A385" s="2"/>
       <c r="B385" s="1"/>
       <c r="D385" s="2"/>
       <c r="E385" s="2"/>
@@ -5402,9 +4834,7 @@
       <c r="J385" s="2"/>
     </row>
     <row r="386" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A386" s="2">
-        <v>2408</v>
-      </c>
+      <c r="A386" s="2"/>
       <c r="B386" s="1"/>
       <c r="D386" s="2"/>
       <c r="E386" s="2"/>
@@ -5415,9 +4845,7 @@
       <c r="J386" s="2"/>
     </row>
     <row r="387" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A387" s="2">
-        <v>2409</v>
-      </c>
+      <c r="A387" s="2"/>
       <c r="B387" s="1"/>
       <c r="D387" s="2"/>
       <c r="E387" s="2"/>
@@ -5428,9 +4856,7 @@
       <c r="J387" s="2"/>
     </row>
     <row r="388" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A388" s="2">
-        <v>2410</v>
-      </c>
+      <c r="A388" s="2"/>
       <c r="B388" s="1"/>
       <c r="D388" s="2"/>
       <c r="E388" s="2"/>
@@ -5441,9 +4867,7 @@
       <c r="J388" s="2"/>
     </row>
     <row r="389" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A389" s="2">
-        <v>2411</v>
-      </c>
+      <c r="A389" s="2"/>
       <c r="B389" s="1"/>
       <c r="D389" s="2"/>
       <c r="E389" s="2"/>
@@ -5454,9 +4878,7 @@
       <c r="J389" s="2"/>
     </row>
     <row r="390" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A390" s="2">
-        <v>2412</v>
-      </c>
+      <c r="A390" s="2"/>
       <c r="B390" s="1"/>
       <c r="D390" s="2"/>
       <c r="E390" s="2"/>
@@ -5467,9 +4889,7 @@
       <c r="J390" s="2"/>
     </row>
     <row r="391" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A391" s="2">
-        <v>2413</v>
-      </c>
+      <c r="A391" s="2"/>
       <c r="B391" s="1"/>
       <c r="D391" s="2"/>
       <c r="E391" s="2"/>
@@ -5480,9 +4900,7 @@
       <c r="J391" s="2"/>
     </row>
     <row r="392" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A392" s="2">
-        <v>2414</v>
-      </c>
+      <c r="A392" s="2"/>
       <c r="B392" s="1"/>
       <c r="D392" s="2"/>
       <c r="E392" s="2"/>
@@ -5493,9 +4911,7 @@
       <c r="J392" s="2"/>
     </row>
     <row r="393" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A393" s="2">
-        <v>2415</v>
-      </c>
+      <c r="A393" s="2"/>
       <c r="B393" s="1"/>
       <c r="D393" s="2"/>
       <c r="E393" s="2"/>
@@ -5506,9 +4922,7 @@
       <c r="J393" s="2"/>
     </row>
     <row r="394" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A394" s="2">
-        <v>2416</v>
-      </c>
+      <c r="A394" s="2"/>
       <c r="B394" s="1"/>
       <c r="D394" s="2"/>
       <c r="E394" s="2"/>
@@ -5519,9 +4933,7 @@
       <c r="J394" s="2"/>
     </row>
     <row r="395" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A395" s="2">
-        <v>2417</v>
-      </c>
+      <c r="A395" s="2"/>
       <c r="B395" s="1"/>
       <c r="D395" s="2"/>
       <c r="E395" s="2"/>
@@ -5532,9 +4944,7 @@
       <c r="J395" s="2"/>
     </row>
     <row r="396" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A396" s="2">
-        <v>2418</v>
-      </c>
+      <c r="A396" s="2"/>
       <c r="B396" s="1"/>
       <c r="D396" s="2"/>
       <c r="E396" s="2"/>
@@ -5545,9 +4955,7 @@
       <c r="J396" s="2"/>
     </row>
     <row r="397" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A397" s="2">
-        <v>2419</v>
-      </c>
+      <c r="A397" s="2"/>
       <c r="B397" s="1"/>
       <c r="D397" s="2"/>
       <c r="E397" s="2"/>
@@ -5558,9 +4966,7 @@
       <c r="J397" s="2"/>
     </row>
     <row r="398" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A398" s="2">
-        <v>2420</v>
-      </c>
+      <c r="A398" s="2"/>
       <c r="B398" s="1"/>
       <c r="D398" s="2"/>
       <c r="E398" s="2"/>
@@ -5571,9 +4977,7 @@
       <c r="J398" s="2"/>
     </row>
     <row r="399" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A399" s="2">
-        <v>2421</v>
-      </c>
+      <c r="A399" s="2"/>
       <c r="B399" s="1"/>
       <c r="D399" s="2"/>
       <c r="E399" s="2"/>
@@ -5584,9 +4988,7 @@
       <c r="J399" s="2"/>
     </row>
     <row r="400" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A400" s="2">
-        <v>2422</v>
-      </c>
+      <c r="A400" s="2"/>
       <c r="B400" s="1"/>
       <c r="D400" s="2"/>
       <c r="E400" s="2"/>
@@ -5597,9 +4999,7 @@
       <c r="J400" s="2"/>
     </row>
     <row r="401" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A401" s="2">
-        <v>2423</v>
-      </c>
+      <c r="A401" s="2"/>
       <c r="B401" s="1"/>
       <c r="D401" s="2"/>
       <c r="E401" s="2"/>
@@ -5610,9 +5010,7 @@
       <c r="J401" s="2"/>
     </row>
     <row r="402" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A402" s="2">
-        <v>2424</v>
-      </c>
+      <c r="A402" s="2"/>
       <c r="B402" s="1"/>
       <c r="D402" s="2"/>
       <c r="E402" s="2"/>
@@ -5623,9 +5021,7 @@
       <c r="J402" s="2"/>
     </row>
     <row r="403" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A403" s="2">
-        <v>2425</v>
-      </c>
+      <c r="A403" s="2"/>
       <c r="B403" s="1"/>
       <c r="D403" s="2"/>
       <c r="E403" s="2"/>
@@ -5636,9 +5032,7 @@
       <c r="J403" s="2"/>
     </row>
     <row r="404" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A404" s="2">
-        <v>2426</v>
-      </c>
+      <c r="A404" s="2"/>
       <c r="B404" s="1"/>
       <c r="D404" s="2"/>
       <c r="E404" s="2"/>
@@ -5649,9 +5043,7 @@
       <c r="J404" s="2"/>
     </row>
     <row r="405" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A405" s="2">
-        <v>2427</v>
-      </c>
+      <c r="A405" s="2"/>
       <c r="B405" s="1"/>
       <c r="D405" s="2"/>
       <c r="E405" s="2"/>
@@ -5662,9 +5054,7 @@
       <c r="J405" s="2"/>
     </row>
     <row r="406" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A406" s="2">
-        <v>2428</v>
-      </c>
+      <c r="A406" s="2"/>
       <c r="B406" s="1"/>
       <c r="D406" s="2"/>
       <c r="E406" s="2"/>
@@ -5675,9 +5065,7 @@
       <c r="J406" s="2"/>
     </row>
     <row r="407" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A407" s="2">
-        <v>2429</v>
-      </c>
+      <c r="A407" s="2"/>
       <c r="B407" s="1"/>
       <c r="D407" s="2"/>
       <c r="E407" s="2"/>
@@ -5688,9 +5076,7 @@
       <c r="J407" s="2"/>
     </row>
     <row r="408" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A408" s="2">
-        <v>2430</v>
-      </c>
+      <c r="A408" s="2"/>
       <c r="B408" s="1"/>
       <c r="D408" s="2"/>
       <c r="E408" s="2"/>
@@ -5701,9 +5087,7 @@
       <c r="J408" s="2"/>
     </row>
     <row r="409" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A409" s="2">
-        <v>2431</v>
-      </c>
+      <c r="A409" s="2"/>
       <c r="B409" s="1"/>
       <c r="D409" s="2"/>
       <c r="E409" s="2"/>
@@ -5714,9 +5098,7 @@
       <c r="J409" s="2"/>
     </row>
     <row r="410" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A410" s="2">
-        <v>2432</v>
-      </c>
+      <c r="A410" s="2"/>
       <c r="B410" s="1"/>
       <c r="D410" s="2"/>
       <c r="E410" s="2"/>
@@ -5727,9 +5109,7 @@
       <c r="J410" s="2"/>
     </row>
     <row r="411" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A411" s="2">
-        <v>2433</v>
-      </c>
+      <c r="A411" s="2"/>
       <c r="B411" s="1"/>
       <c r="D411" s="2"/>
       <c r="E411" s="2"/>
@@ -5740,9 +5120,7 @@
       <c r="J411" s="2"/>
     </row>
     <row r="412" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A412" s="2">
-        <v>2434</v>
-      </c>
+      <c r="A412" s="2"/>
       <c r="B412" s="1"/>
       <c r="D412" s="2"/>
       <c r="E412" s="2"/>
@@ -5753,9 +5131,7 @@
       <c r="J412" s="2"/>
     </row>
     <row r="413" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A413" s="2">
-        <v>2435</v>
-      </c>
+      <c r="A413" s="2"/>
       <c r="B413" s="1"/>
       <c r="D413" s="2"/>
       <c r="E413" s="2"/>
@@ -5766,9 +5142,7 @@
       <c r="J413" s="2"/>
     </row>
     <row r="414" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A414" s="2">
-        <v>2436</v>
-      </c>
+      <c r="A414" s="2"/>
       <c r="B414" s="1"/>
       <c r="D414" s="2"/>
       <c r="E414" s="2"/>
@@ -5779,9 +5153,7 @@
       <c r="J414" s="2"/>
     </row>
     <row r="415" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A415" s="2">
-        <v>2437</v>
-      </c>
+      <c r="A415" s="2"/>
       <c r="B415" s="1"/>
       <c r="D415" s="2"/>
       <c r="E415" s="2"/>
@@ -5792,9 +5164,7 @@
       <c r="J415" s="2"/>
     </row>
     <row r="416" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A416" s="2">
-        <v>2438</v>
-      </c>
+      <c r="A416" s="2"/>
       <c r="B416" s="1"/>
       <c r="D416" s="2"/>
       <c r="E416" s="2"/>
@@ -5805,9 +5175,7 @@
       <c r="J416" s="2"/>
     </row>
     <row r="417" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A417" s="2">
-        <v>2439</v>
-      </c>
+      <c r="A417" s="2"/>
       <c r="B417" s="1"/>
       <c r="D417" s="2"/>
       <c r="E417" s="2"/>
@@ -5818,9 +5186,7 @@
       <c r="J417" s="2"/>
     </row>
     <row r="418" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A418" s="2">
-        <v>2440</v>
-      </c>
+      <c r="A418" s="2"/>
       <c r="B418" s="1"/>
       <c r="D418" s="2"/>
       <c r="E418" s="2"/>
@@ -5831,9 +5197,7 @@
       <c r="J418" s="2"/>
     </row>
     <row r="419" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A419" s="2">
-        <v>2441</v>
-      </c>
+      <c r="A419" s="2"/>
       <c r="B419" s="1"/>
       <c r="D419" s="2"/>
       <c r="E419" s="2"/>
@@ -5844,9 +5208,7 @@
       <c r="J419" s="2"/>
     </row>
     <row r="420" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A420" s="2">
-        <v>2442</v>
-      </c>
+      <c r="A420" s="2"/>
       <c r="B420" s="1"/>
       <c r="D420" s="2"/>
       <c r="E420" s="2"/>
@@ -5857,9 +5219,7 @@
       <c r="J420" s="2"/>
     </row>
     <row r="421" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A421" s="2">
-        <v>2443</v>
-      </c>
+      <c r="A421" s="2"/>
       <c r="B421" s="1"/>
       <c r="D421" s="2"/>
       <c r="E421" s="2"/>
@@ -5870,9 +5230,7 @@
       <c r="J421" s="2"/>
     </row>
     <row r="422" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A422" s="2">
-        <v>2444</v>
-      </c>
+      <c r="A422" s="2"/>
       <c r="B422" s="1"/>
       <c r="D422" s="2"/>
       <c r="E422" s="2"/>
@@ -5883,9 +5241,7 @@
       <c r="J422" s="2"/>
     </row>
     <row r="423" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A423" s="2">
-        <v>2445</v>
-      </c>
+      <c r="A423" s="2"/>
       <c r="B423" s="1"/>
       <c r="D423" s="2"/>
       <c r="E423" s="2"/>
@@ -5896,9 +5252,7 @@
       <c r="J423" s="2"/>
     </row>
     <row r="424" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A424" s="2">
-        <v>2446</v>
-      </c>
+      <c r="A424" s="2"/>
       <c r="B424" s="1"/>
       <c r="D424" s="2"/>
       <c r="E424" s="2"/>
@@ -5909,9 +5263,7 @@
       <c r="J424" s="2"/>
     </row>
     <row r="425" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A425" s="2">
-        <v>2447</v>
-      </c>
+      <c r="A425" s="2"/>
       <c r="B425" s="1"/>
       <c r="D425" s="2"/>
       <c r="E425" s="2"/>
@@ -5922,9 +5274,7 @@
       <c r="J425" s="2"/>
     </row>
     <row r="426" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A426" s="2">
-        <v>2448</v>
-      </c>
+      <c r="A426" s="2"/>
       <c r="B426" s="1"/>
       <c r="D426" s="2"/>
       <c r="E426" s="2"/>
@@ -5935,9 +5285,7 @@
       <c r="J426" s="2"/>
     </row>
     <row r="427" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A427" s="2">
-        <v>2449</v>
-      </c>
+      <c r="A427" s="2"/>
       <c r="B427" s="1"/>
       <c r="D427" s="2"/>
       <c r="E427" s="2"/>
@@ -5948,9 +5296,7 @@
       <c r="J427" s="2"/>
     </row>
     <row r="428" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A428" s="2">
-        <v>2450</v>
-      </c>
+      <c r="A428" s="2"/>
       <c r="B428" s="1"/>
       <c r="D428" s="2"/>
       <c r="E428" s="2"/>
@@ -5961,9 +5307,7 @@
       <c r="J428" s="2"/>
     </row>
     <row r="429" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A429" s="2">
-        <v>2451</v>
-      </c>
+      <c r="A429" s="2"/>
       <c r="B429" s="1"/>
       <c r="D429" s="2"/>
       <c r="E429" s="2"/>
@@ -5974,9 +5318,7 @@
       <c r="J429" s="2"/>
     </row>
     <row r="430" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A430" s="2">
-        <v>2452</v>
-      </c>
+      <c r="A430" s="2"/>
       <c r="B430" s="1"/>
       <c r="D430" s="2"/>
       <c r="E430" s="2"/>
@@ -5987,9 +5329,7 @@
       <c r="J430" s="2"/>
     </row>
     <row r="431" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A431" s="2">
-        <v>2453</v>
-      </c>
+      <c r="A431" s="2"/>
       <c r="B431" s="1"/>
       <c r="D431" s="2"/>
       <c r="E431" s="2"/>
@@ -6000,9 +5340,7 @@
       <c r="J431" s="2"/>
     </row>
     <row r="432" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A432" s="2">
-        <v>2454</v>
-      </c>
+      <c r="A432" s="2"/>
       <c r="B432" s="1"/>
       <c r="D432" s="2"/>
       <c r="E432" s="2"/>
@@ -6013,9 +5351,7 @@
       <c r="J432" s="2"/>
     </row>
     <row r="433" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A433" s="2">
-        <v>2455</v>
-      </c>
+      <c r="A433" s="2"/>
       <c r="B433" s="1"/>
       <c r="D433" s="2"/>
       <c r="E433" s="2"/>
@@ -6026,9 +5362,7 @@
       <c r="J433" s="2"/>
     </row>
     <row r="434" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A434" s="2">
-        <v>2456</v>
-      </c>
+      <c r="A434" s="2"/>
       <c r="B434" s="1"/>
       <c r="D434" s="2"/>
       <c r="E434" s="2"/>
@@ -6039,9 +5373,7 @@
       <c r="J434" s="2"/>
     </row>
     <row r="435" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A435" s="2">
-        <v>2457</v>
-      </c>
+      <c r="A435" s="2"/>
       <c r="B435" s="1"/>
       <c r="D435" s="2"/>
       <c r="E435" s="2"/>
@@ -6052,9 +5384,7 @@
       <c r="J435" s="2"/>
     </row>
     <row r="436" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A436" s="2">
-        <v>2458</v>
-      </c>
+      <c r="A436" s="2"/>
       <c r="B436" s="1"/>
       <c r="D436" s="2"/>
       <c r="E436" s="2"/>
@@ -6065,9 +5395,7 @@
       <c r="J436" s="2"/>
     </row>
     <row r="437" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A437" s="2">
-        <v>2459</v>
-      </c>
+      <c r="A437" s="2"/>
       <c r="B437" s="1"/>
       <c r="D437" s="2"/>
       <c r="E437" s="2"/>
@@ -6078,9 +5406,7 @@
       <c r="J437" s="2"/>
     </row>
     <row r="438" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A438" s="2">
-        <v>2460</v>
-      </c>
+      <c r="A438" s="2"/>
       <c r="B438" s="1"/>
       <c r="D438" s="2"/>
       <c r="E438" s="2"/>
@@ -6091,9 +5417,7 @@
       <c r="J438" s="2"/>
     </row>
     <row r="439" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A439" s="2">
-        <v>2461</v>
-      </c>
+      <c r="A439" s="2"/>
       <c r="B439" s="1"/>
       <c r="D439" s="2"/>
       <c r="E439" s="2"/>
@@ -6104,9 +5428,7 @@
       <c r="J439" s="2"/>
     </row>
     <row r="440" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A440" s="2">
-        <v>2462</v>
-      </c>
+      <c r="A440" s="2"/>
       <c r="B440" s="1"/>
       <c r="D440" s="2"/>
       <c r="E440" s="2"/>
@@ -6117,9 +5439,7 @@
       <c r="J440" s="2"/>
     </row>
     <row r="441" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A441" s="2">
-        <v>2463</v>
-      </c>
+      <c r="A441" s="2"/>
       <c r="B441" s="1"/>
       <c r="D441" s="2"/>
       <c r="E441" s="2"/>
@@ -6130,9 +5450,7 @@
       <c r="J441" s="2"/>
     </row>
     <row r="442" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A442" s="2">
-        <v>2464</v>
-      </c>
+      <c r="A442" s="2"/>
       <c r="B442" s="1"/>
       <c r="D442" s="2"/>
       <c r="E442" s="2"/>
@@ -6143,9 +5461,7 @@
       <c r="J442" s="2"/>
     </row>
     <row r="443" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A443" s="2">
-        <v>2465</v>
-      </c>
+      <c r="A443" s="2"/>
       <c r="B443" s="1"/>
       <c r="D443" s="2"/>
       <c r="E443" s="2"/>
@@ -6156,9 +5472,7 @@
       <c r="J443" s="2"/>
     </row>
     <row r="444" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A444" s="2">
-        <v>2466</v>
-      </c>
+      <c r="A444" s="2"/>
       <c r="B444" s="1"/>
       <c r="D444" s="2"/>
       <c r="E444" s="2"/>
@@ -6169,9 +5483,7 @@
       <c r="J444" s="2"/>
     </row>
     <row r="445" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A445" s="2">
-        <v>2467</v>
-      </c>
+      <c r="A445" s="2"/>
       <c r="B445" s="1"/>
       <c r="D445" s="2"/>
       <c r="E445" s="2"/>
@@ -6182,9 +5494,7 @@
       <c r="J445" s="2"/>
     </row>
     <row r="446" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A446" s="2">
-        <v>2468</v>
-      </c>
+      <c r="A446" s="2"/>
       <c r="B446" s="1"/>
       <c r="D446" s="2"/>
       <c r="E446" s="2"/>
@@ -6195,9 +5505,7 @@
       <c r="J446" s="2"/>
     </row>
     <row r="447" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A447" s="2">
-        <v>2469</v>
-      </c>
+      <c r="A447" s="2"/>
       <c r="B447" s="1"/>
       <c r="D447" s="2"/>
       <c r="E447" s="2"/>
@@ -6208,9 +5516,7 @@
       <c r="J447" s="2"/>
     </row>
     <row r="448" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A448" s="2">
-        <v>2470</v>
-      </c>
+      <c r="A448" s="2"/>
       <c r="B448" s="1"/>
       <c r="D448" s="2"/>
       <c r="E448" s="2"/>
@@ -6221,9 +5527,7 @@
       <c r="J448" s="2"/>
     </row>
     <row r="449" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A449" s="2">
-        <v>2471</v>
-      </c>
+      <c r="A449" s="2"/>
       <c r="B449" s="1"/>
       <c r="D449" s="2"/>
       <c r="E449" s="2"/>
@@ -6234,9 +5538,7 @@
       <c r="J449" s="2"/>
     </row>
     <row r="450" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A450" s="2">
-        <v>2472</v>
-      </c>
+      <c r="A450" s="2"/>
       <c r="B450" s="1"/>
       <c r="D450" s="2"/>
       <c r="E450" s="2"/>
@@ -6247,9 +5549,7 @@
       <c r="J450" s="2"/>
     </row>
     <row r="451" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A451" s="2">
-        <v>2473</v>
-      </c>
+      <c r="A451" s="2"/>
       <c r="B451" s="1"/>
       <c r="D451" s="2"/>
       <c r="E451" s="2"/>
@@ -6260,9 +5560,7 @@
       <c r="J451" s="2"/>
     </row>
     <row r="452" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A452" s="2">
-        <v>2474</v>
-      </c>
+      <c r="A452" s="2"/>
       <c r="B452" s="1"/>
       <c r="D452" s="2"/>
       <c r="E452" s="2"/>
@@ -6273,9 +5571,7 @@
       <c r="J452" s="2"/>
     </row>
     <row r="453" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A453" s="2">
-        <v>2475</v>
-      </c>
+      <c r="A453" s="2"/>
       <c r="B453" s="1"/>
       <c r="D453" s="2"/>
       <c r="E453" s="2"/>
@@ -6286,9 +5582,7 @@
       <c r="J453" s="2"/>
     </row>
     <row r="454" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A454" s="2">
-        <v>2476</v>
-      </c>
+      <c r="A454" s="2"/>
       <c r="B454" s="1"/>
       <c r="D454" s="2"/>
       <c r="E454" s="2"/>
@@ -6299,9 +5593,7 @@
       <c r="J454" s="2"/>
     </row>
     <row r="455" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A455" s="2">
-        <v>2477</v>
-      </c>
+      <c r="A455" s="2"/>
       <c r="B455" s="1"/>
       <c r="D455" s="2"/>
       <c r="E455" s="2"/>
@@ -6312,9 +5604,7 @@
       <c r="J455" s="2"/>
     </row>
     <row r="456" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A456" s="2">
-        <v>2478</v>
-      </c>
+      <c r="A456" s="2"/>
       <c r="B456" s="1"/>
       <c r="D456" s="2"/>
       <c r="E456" s="2"/>
@@ -6325,9 +5615,7 @@
       <c r="J456" s="2"/>
     </row>
     <row r="457" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A457" s="2">
-        <v>2479</v>
-      </c>
+      <c r="A457" s="2"/>
       <c r="B457" s="1"/>
       <c r="D457" s="2"/>
       <c r="E457" s="2"/>
@@ -6338,9 +5626,7 @@
       <c r="J457" s="2"/>
     </row>
     <row r="458" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A458" s="2">
-        <v>2480</v>
-      </c>
+      <c r="A458" s="2"/>
       <c r="B458" s="1"/>
       <c r="D458" s="2"/>
       <c r="E458" s="2"/>
@@ -6351,9 +5637,7 @@
       <c r="J458" s="2"/>
     </row>
     <row r="459" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A459" s="2">
-        <v>2481</v>
-      </c>
+      <c r="A459" s="2"/>
       <c r="B459" s="1"/>
       <c r="D459" s="2"/>
       <c r="E459" s="2"/>
@@ -6364,9 +5648,7 @@
       <c r="J459" s="2"/>
     </row>
     <row r="460" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A460" s="2">
-        <v>2482</v>
-      </c>
+      <c r="A460" s="2"/>
       <c r="B460" s="1"/>
       <c r="D460" s="2"/>
       <c r="E460" s="2"/>
@@ -6377,9 +5659,7 @@
       <c r="J460" s="2"/>
     </row>
     <row r="461" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A461" s="2">
-        <v>2483</v>
-      </c>
+      <c r="A461" s="2"/>
       <c r="B461" s="1"/>
       <c r="D461" s="2"/>
       <c r="E461" s="2"/>
@@ -6390,9 +5670,7 @@
       <c r="J461" s="2"/>
     </row>
     <row r="462" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A462" s="2">
-        <v>2484</v>
-      </c>
+      <c r="A462" s="2"/>
       <c r="B462" s="1"/>
       <c r="D462" s="2"/>
       <c r="E462" s="2"/>
@@ -6403,9 +5681,7 @@
       <c r="J462" s="2"/>
     </row>
     <row r="463" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A463" s="2">
-        <v>2485</v>
-      </c>
+      <c r="A463" s="2"/>
       <c r="B463" s="1"/>
       <c r="D463" s="2"/>
       <c r="E463" s="2"/>
@@ -6416,9 +5692,7 @@
       <c r="J463" s="2"/>
     </row>
     <row r="464" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A464" s="2">
-        <v>2486</v>
-      </c>
+      <c r="A464" s="2"/>
       <c r="B464" s="1"/>
       <c r="D464" s="2"/>
       <c r="E464" s="2"/>
@@ -6429,9 +5703,7 @@
       <c r="J464" s="2"/>
     </row>
     <row r="465" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A465" s="2">
-        <v>2487</v>
-      </c>
+      <c r="A465" s="2"/>
       <c r="B465" s="1"/>
       <c r="D465" s="2"/>
       <c r="E465" s="2"/>
@@ -6442,9 +5714,7 @@
       <c r="J465" s="2"/>
     </row>
     <row r="466" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A466" s="2">
-        <v>2488</v>
-      </c>
+      <c r="A466" s="2"/>
       <c r="B466" s="1"/>
       <c r="D466" s="2"/>
       <c r="E466" s="2"/>
@@ -6455,9 +5725,7 @@
       <c r="J466" s="2"/>
     </row>
     <row r="467" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A467" s="2">
-        <v>2489</v>
-      </c>
+      <c r="A467" s="2"/>
       <c r="B467" s="1"/>
       <c r="D467" s="2"/>
       <c r="E467" s="2"/>
@@ -6468,9 +5736,7 @@
       <c r="J467" s="2"/>
     </row>
     <row r="468" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A468" s="2">
-        <v>2490</v>
-      </c>
+      <c r="A468" s="2"/>
       <c r="B468" s="1"/>
       <c r="D468" s="2"/>
       <c r="E468" s="2"/>
@@ -6481,9 +5747,7 @@
       <c r="J468" s="2"/>
     </row>
     <row r="469" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A469" s="2">
-        <v>2491</v>
-      </c>
+      <c r="A469" s="2"/>
       <c r="B469" s="1"/>
       <c r="D469" s="2"/>
       <c r="E469" s="2"/>
@@ -6494,9 +5758,7 @@
       <c r="J469" s="2"/>
     </row>
     <row r="470" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A470" s="2">
-        <v>2492</v>
-      </c>
+      <c r="A470" s="2"/>
       <c r="B470" s="1"/>
       <c r="D470" s="2"/>
       <c r="E470" s="2"/>
@@ -6507,9 +5769,7 @@
       <c r="J470" s="2"/>
     </row>
     <row r="471" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A471" s="2">
-        <v>2493</v>
-      </c>
+      <c r="A471" s="2"/>
       <c r="B471" s="1"/>
       <c r="D471" s="2"/>
       <c r="E471" s="2"/>
@@ -6520,9 +5780,7 @@
       <c r="J471" s="2"/>
     </row>
     <row r="472" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A472" s="2">
-        <v>2494</v>
-      </c>
+      <c r="A472" s="2"/>
       <c r="B472" s="1"/>
       <c r="D472" s="2"/>
       <c r="E472" s="2"/>
@@ -6533,9 +5791,7 @@
       <c r="J472" s="2"/>
     </row>
     <row r="473" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A473" s="2">
-        <v>2495</v>
-      </c>
+      <c r="A473" s="2"/>
       <c r="B473" s="1"/>
       <c r="D473" s="2"/>
       <c r="E473" s="2"/>
@@ -6546,9 +5802,7 @@
       <c r="J473" s="2"/>
     </row>
     <row r="474" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A474" s="2">
-        <v>2496</v>
-      </c>
+      <c r="A474" s="2"/>
       <c r="B474" s="1"/>
       <c r="D474" s="2"/>
       <c r="E474" s="2"/>
@@ -6559,9 +5813,7 @@
       <c r="J474" s="2"/>
     </row>
     <row r="475" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A475" s="2">
-        <v>2497</v>
-      </c>
+      <c r="A475" s="2"/>
       <c r="B475" s="1"/>
       <c r="D475" s="2"/>
       <c r="E475" s="2"/>
@@ -6572,9 +5824,7 @@
       <c r="J475" s="2"/>
     </row>
     <row r="476" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A476" s="2">
-        <v>2498</v>
-      </c>
+      <c r="A476" s="2"/>
       <c r="B476" s="1"/>
       <c r="D476" s="2"/>
       <c r="E476" s="2"/>
@@ -6585,9 +5835,7 @@
       <c r="J476" s="2"/>
     </row>
     <row r="477" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A477" s="2">
-        <v>2499</v>
-      </c>
+      <c r="A477" s="2"/>
       <c r="B477" s="1"/>
       <c r="D477" s="2"/>
       <c r="E477" s="2"/>
@@ -6598,9 +5846,7 @@
       <c r="J477" s="2"/>
     </row>
     <row r="478" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A478" s="2">
-        <v>2500</v>
-      </c>
+      <c r="A478" s="2"/>
       <c r="B478" s="1"/>
       <c r="D478" s="2"/>
       <c r="E478" s="2"/>
@@ -6611,9 +5857,7 @@
       <c r="J478" s="2"/>
     </row>
     <row r="479" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A479" s="2">
-        <v>2501</v>
-      </c>
+      <c r="A479" s="2"/>
       <c r="B479" s="1"/>
       <c r="D479" s="2"/>
       <c r="E479" s="2"/>
@@ -6624,9 +5868,7 @@
       <c r="J479" s="2"/>
     </row>
     <row r="480" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A480" s="2">
-        <v>2502</v>
-      </c>
+      <c r="A480" s="2"/>
       <c r="B480" s="1"/>
       <c r="D480" s="2"/>
       <c r="E480" s="2"/>
@@ -6637,9 +5879,7 @@
       <c r="J480" s="2"/>
     </row>
     <row r="481" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A481" s="2">
-        <v>2503</v>
-      </c>
+      <c r="A481" s="2"/>
       <c r="B481" s="1"/>
       <c r="D481" s="2"/>
       <c r="E481" s="2"/>
@@ -6650,9 +5890,7 @@
       <c r="J481" s="2"/>
     </row>
     <row r="482" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A482" s="2">
-        <v>2504</v>
-      </c>
+      <c r="A482" s="2"/>
       <c r="B482" s="1"/>
       <c r="D482" s="2"/>
       <c r="E482" s="2"/>
@@ -6663,9 +5901,7 @@
       <c r="J482" s="2"/>
     </row>
     <row r="483" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A483" s="2">
-        <v>2505</v>
-      </c>
+      <c r="A483" s="2"/>
       <c r="B483" s="1"/>
       <c r="D483" s="2"/>
       <c r="E483" s="2"/>
@@ -6676,9 +5912,7 @@
       <c r="J483" s="2"/>
     </row>
     <row r="484" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A484" s="2">
-        <v>2506</v>
-      </c>
+      <c r="A484" s="2"/>
       <c r="B484" s="1"/>
       <c r="D484" s="2"/>
       <c r="E484" s="2"/>
@@ -6689,9 +5923,7 @@
       <c r="J484" s="2"/>
     </row>
     <row r="485" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A485" s="2">
-        <v>2507</v>
-      </c>
+      <c r="A485" s="2"/>
       <c r="B485" s="1"/>
       <c r="D485" s="2"/>
       <c r="E485" s="2"/>
@@ -6702,9 +5934,7 @@
       <c r="J485" s="2"/>
     </row>
     <row r="486" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A486" s="2">
-        <v>2508</v>
-      </c>
+      <c r="A486" s="2"/>
       <c r="B486" s="1"/>
       <c r="D486" s="2"/>
       <c r="E486" s="2"/>
@@ -6715,9 +5945,7 @@
       <c r="J486" s="2"/>
     </row>
     <row r="487" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A487" s="2">
-        <v>2509</v>
-      </c>
+      <c r="A487" s="2"/>
       <c r="B487" s="1"/>
       <c r="D487" s="2"/>
       <c r="E487" s="2"/>
@@ -6728,9 +5956,7 @@
       <c r="J487" s="2"/>
     </row>
     <row r="488" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A488" s="2">
-        <v>2510</v>
-      </c>
+      <c r="A488" s="2"/>
       <c r="B488" s="1"/>
       <c r="D488" s="2"/>
       <c r="E488" s="2"/>
@@ -6741,9 +5967,7 @@
       <c r="J488" s="2"/>
     </row>
     <row r="489" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A489" s="2">
-        <v>2511</v>
-      </c>
+      <c r="A489" s="2"/>
       <c r="B489" s="1"/>
       <c r="D489" s="2"/>
       <c r="E489" s="2"/>
@@ -6754,9 +5978,7 @@
       <c r="J489" s="2"/>
     </row>
     <row r="490" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A490" s="2">
-        <v>2512</v>
-      </c>
+      <c r="A490" s="2"/>
       <c r="B490" s="1"/>
       <c r="D490" s="2"/>
       <c r="E490" s="2"/>
@@ -6767,9 +5989,7 @@
       <c r="J490" s="2"/>
     </row>
     <row r="491" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A491" s="2">
-        <v>2513</v>
-      </c>
+      <c r="A491" s="2"/>
       <c r="B491" s="1"/>
       <c r="D491" s="2"/>
       <c r="E491" s="2"/>
@@ -6780,9 +6000,7 @@
       <c r="J491" s="2"/>
     </row>
     <row r="492" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A492" s="2">
-        <v>2514</v>
-      </c>
+      <c r="A492" s="2"/>
       <c r="B492" s="1"/>
       <c r="D492" s="2"/>
       <c r="E492" s="2"/>
@@ -6793,9 +6011,7 @@
       <c r="J492" s="2"/>
     </row>
     <row r="493" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A493" s="2">
-        <v>2515</v>
-      </c>
+      <c r="A493" s="2"/>
       <c r="B493" s="1"/>
       <c r="D493" s="2"/>
       <c r="E493" s="2"/>
@@ -6806,9 +6022,7 @@
       <c r="J493" s="2"/>
     </row>
     <row r="494" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A494" s="2">
-        <v>2516</v>
-      </c>
+      <c r="A494" s="2"/>
       <c r="B494" s="1"/>
       <c r="D494" s="2"/>
       <c r="E494" s="2"/>
@@ -6819,9 +6033,7 @@
       <c r="J494" s="2"/>
     </row>
     <row r="495" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A495" s="2">
-        <v>2517</v>
-      </c>
+      <c r="A495" s="2"/>
       <c r="B495" s="1"/>
       <c r="D495" s="2"/>
       <c r="E495" s="2"/>
@@ -6832,9 +6044,7 @@
       <c r="J495" s="2"/>
     </row>
     <row r="496" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A496" s="2">
-        <v>2518</v>
-      </c>
+      <c r="A496" s="2"/>
       <c r="B496" s="1"/>
       <c r="D496" s="2"/>
       <c r="E496" s="2"/>
@@ -6845,9 +6055,7 @@
       <c r="J496" s="2"/>
     </row>
     <row r="497" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A497" s="2">
-        <v>2519</v>
-      </c>
+      <c r="A497" s="2"/>
       <c r="B497" s="1"/>
       <c r="D497" s="2"/>
       <c r="E497" s="2"/>
@@ -6858,9 +6066,7 @@
       <c r="J497" s="2"/>
     </row>
     <row r="498" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A498" s="2">
-        <v>2520</v>
-      </c>
+      <c r="A498" s="2"/>
       <c r="B498" s="1"/>
       <c r="D498" s="2"/>
       <c r="E498" s="2"/>
@@ -6871,9 +6077,7 @@
       <c r="J498" s="2"/>
     </row>
     <row r="499" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A499" s="2">
-        <v>2521</v>
-      </c>
+      <c r="A499" s="2"/>
       <c r="B499" s="1"/>
       <c r="D499" s="2"/>
       <c r="E499" s="2"/>
@@ -6884,9 +6088,7 @@
       <c r="J499" s="2"/>
     </row>
     <row r="500" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A500" s="2">
-        <v>2522</v>
-      </c>
+      <c r="A500" s="2"/>
       <c r="B500" s="1"/>
       <c r="D500" s="2"/>
       <c r="E500" s="2"/>
@@ -6897,9 +6099,7 @@
       <c r="J500" s="2"/>
     </row>
     <row r="501" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A501" s="2">
-        <v>2523</v>
-      </c>
+      <c r="A501" s="2"/>
       <c r="B501" s="1"/>
       <c r="D501" s="2"/>
       <c r="E501" s="2"/>
@@ -6910,9 +6110,7 @@
       <c r="J501" s="2"/>
     </row>
     <row r="502" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A502" s="2">
-        <v>2524</v>
-      </c>
+      <c r="A502" s="2"/>
       <c r="B502" s="1"/>
       <c r="D502" s="2"/>
       <c r="E502" s="2"/>
@@ -6923,9 +6121,7 @@
       <c r="J502" s="2"/>
     </row>
     <row r="503" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A503" s="2">
-        <v>2525</v>
-      </c>
+      <c r="A503" s="2"/>
       <c r="B503" s="1"/>
       <c r="D503" s="2"/>
       <c r="E503" s="2"/>
@@ -6936,9 +6132,7 @@
       <c r="J503" s="2"/>
     </row>
     <row r="504" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A504" s="2">
-        <v>2526</v>
-      </c>
+      <c r="A504" s="2"/>
       <c r="B504" s="1"/>
     </row>
   </sheetData>

</xml_diff>